<commit_message>
Issue 15: Export the results to a .csv
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -450,13 +450,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-2.39909375345095</v>
+        <v>-2.3991</v>
       </c>
       <c r="C2" t="n">
-        <v>62420.4525398934</v>
+        <v>62420.4525</v>
       </c>
       <c r="D2" t="n">
-        <v>0.999969333771425</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -464,13 +464,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.621726438125615</v>
+        <v>-0.6217</v>
       </c>
       <c r="C3" t="n">
-        <v>0.446563396294826</v>
+        <v>0.4466</v>
       </c>
       <c r="D3" t="n">
-        <v>0.163847689793895</v>
+        <v>0.1638</v>
       </c>
     </row>
     <row r="4">
@@ -478,13 +478,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.346837641952026</v>
+        <v>-0.3468</v>
       </c>
       <c r="C4" t="n">
-        <v>0.358494562257901</v>
+        <v>0.3585</v>
       </c>
       <c r="D4" t="n">
-        <v>0.333302290818082</v>
+        <v>0.3333</v>
       </c>
     </row>
     <row r="5">
@@ -492,13 +492,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>3.83220696378058</v>
+        <v>3.8322</v>
       </c>
       <c r="C5" t="n">
-        <v>62420.4525255146</v>
+        <v>62420.4525</v>
       </c>
       <c r="D5" t="n">
-        <v>0.999951015113724</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -506,13 +506,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.415959452875481</v>
+        <v>-0.416</v>
       </c>
       <c r="C6" t="n">
-        <v>83119.3212186157</v>
+        <v>83119.3212</v>
       </c>
       <c r="D6" t="n">
-        <v>0.999996007094133</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -520,13 +520,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.0571973230482257</v>
+        <v>-0.0572</v>
       </c>
       <c r="C7" t="n">
-        <v>80488.0075943448</v>
+        <v>80488.0076</v>
       </c>
       <c r="D7" t="n">
-        <v>0.999999432998004</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -534,13 +534,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>0.775637968087059</v>
+        <v>0.7756</v>
       </c>
       <c r="C8" t="n">
-        <v>92489.6876247333</v>
+        <v>92489.6876</v>
       </c>
       <c r="D8" t="n">
-        <v>0.999993308772303</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -548,13 +548,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>3.81123870903567</v>
+        <v>3.8112</v>
       </c>
       <c r="C9" t="n">
-        <v>62420.4525255564</v>
+        <v>62420.4525</v>
       </c>
       <c r="D9" t="n">
-        <v>0.999951283138802</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -562,13 +562,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>3.74202116607166</v>
+        <v>3.742</v>
       </c>
       <c r="C10" t="n">
-        <v>62420.4525252916</v>
+        <v>62420.4525</v>
       </c>
       <c r="D10" t="n">
-        <v>0.999952167906639</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -576,13 +576,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.317939108720248</v>
+        <v>-0.3179</v>
       </c>
       <c r="C11" t="n">
-        <v>83906.3177659629</v>
+        <v>83906.3178</v>
       </c>
       <c r="D11" t="n">
-        <v>0.999996976643561</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -590,13 +590,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.973735851366318</v>
+        <v>-0.9737</v>
       </c>
       <c r="C12" t="n">
-        <v>1.14334031208868</v>
+        <v>1.1433</v>
       </c>
       <c r="D12" t="n">
-        <v>0.394403487475458</v>
+        <v>0.3944</v>
       </c>
     </row>
     <row r="13">
@@ -604,13 +604,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.69128793957788</v>
+        <v>-1.6913</v>
       </c>
       <c r="C13" t="n">
-        <v>1.56989329119463</v>
+        <v>1.5699</v>
       </c>
       <c r="D13" t="n">
-        <v>0.281334343559962</v>
+        <v>0.2813</v>
       </c>
     </row>
     <row r="14">
@@ -618,13 +618,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.58435939633627</v>
+        <v>-1.5844</v>
       </c>
       <c r="C14" t="n">
-        <v>1.55224082586339</v>
+        <v>1.5522</v>
       </c>
       <c r="D14" t="n">
-        <v>0.307400507066783</v>
+        <v>0.3074</v>
       </c>
     </row>
     <row r="15">
@@ -632,13 +632,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.03566860498879</v>
+        <v>-1.0357</v>
       </c>
       <c r="C15" t="n">
-        <v>1.38946683614383</v>
+        <v>1.3895</v>
       </c>
       <c r="D15" t="n">
-        <v>0.456047331093435</v>
+        <v>0.456</v>
       </c>
     </row>
     <row r="16">
@@ -646,13 +646,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.552095268289528</v>
+        <v>-0.5521</v>
       </c>
       <c r="C16" t="n">
-        <v>1.32275580150065</v>
+        <v>1.3228</v>
       </c>
       <c r="D16" t="n">
-        <v>0.676398572897828</v>
+        <v>0.6764</v>
       </c>
     </row>
     <row r="17">
@@ -660,13 +660,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.178518779772545</v>
+        <v>-0.1785</v>
       </c>
       <c r="C17" t="n">
-        <v>1.26830203636834</v>
+        <v>1.2683</v>
       </c>
       <c r="D17" t="n">
-        <v>0.888064162430655</v>
+        <v>0.8881</v>
       </c>
     </row>
     <row r="18">
@@ -674,13 +674,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.108125524782969</v>
+        <v>-0.1081</v>
       </c>
       <c r="C18" t="n">
-        <v>1.23430033652575</v>
+        <v>1.2343</v>
       </c>
       <c r="D18" t="n">
-        <v>0.930194077165221</v>
+        <v>0.9302</v>
       </c>
     </row>
     <row r="19">
@@ -688,13 +688,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.478542851681695</v>
+        <v>-0.4785</v>
       </c>
       <c r="C19" t="n">
-        <v>1.23744721552008</v>
+        <v>1.2374</v>
       </c>
       <c r="D19" t="n">
-        <v>0.698965144865284</v>
+        <v>0.699</v>
       </c>
     </row>
     <row r="20">
@@ -702,13 +702,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.707018679798631</v>
+        <v>-0.707</v>
       </c>
       <c r="C20" t="n">
-        <v>1.33615055931206</v>
+        <v>1.3362</v>
       </c>
       <c r="D20" t="n">
-        <v>0.596704196078925</v>
+        <v>0.5967</v>
       </c>
     </row>
     <row r="21">
@@ -716,13 +716,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.787972102479502</v>
+        <v>-0.788</v>
       </c>
       <c r="C21" t="n">
-        <v>1.39564683618295</v>
+        <v>1.3956</v>
       </c>
       <c r="D21" t="n">
-        <v>0.572350789285024</v>
+        <v>0.5724</v>
       </c>
     </row>
     <row r="22">
@@ -730,13 +730,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.837547376183614</v>
+        <v>-0.8375</v>
       </c>
       <c r="C22" t="n">
-        <v>1.76436770351332</v>
+        <v>1.7644</v>
       </c>
       <c r="D22" t="n">
-        <v>0.634999998830929</v>
+        <v>0.635</v>
       </c>
     </row>
     <row r="23">
@@ -744,13 +744,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.887078765314423</v>
+        <v>-0.8871</v>
       </c>
       <c r="C23" t="n">
-        <v>2.72866102915728</v>
+        <v>2.7287</v>
       </c>
       <c r="D23" t="n">
-        <v>0.745107867222508</v>
+        <v>0.7451</v>
       </c>
     </row>
     <row r="24">
@@ -758,13 +758,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.644780512481345</v>
+        <v>-0.6448</v>
       </c>
       <c r="C24" t="n">
-        <v>0.208200131659363</v>
+        <v>0.2082</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00195538326513929</v>
+        <v>0.002</v>
       </c>
     </row>
   </sheetData>
@@ -800,13 +800,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>1.87344337189236</v>
+        <v>1.8734</v>
       </c>
       <c r="C2" t="n">
-        <v>0.700792680433909</v>
+        <v>0.7008</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00751044791351729</v>
+        <v>0.0075</v>
       </c>
     </row>
     <row r="3">
@@ -814,13 +814,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.183062160944288</v>
+        <v>0.1831</v>
       </c>
       <c r="C3" t="n">
-        <v>0.183410500628311</v>
+        <v>0.1834</v>
       </c>
       <c r="D3" t="n">
-        <v>0.31823049932207</v>
+        <v>0.3182</v>
       </c>
     </row>
     <row r="4">
@@ -828,13 +828,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0930228721293085</v>
+        <v>0.093</v>
       </c>
       <c r="C4" t="n">
-        <v>0.170832307431283</v>
+        <v>0.1708</v>
       </c>
       <c r="D4" t="n">
-        <v>0.586078598863253</v>
+        <v>0.5861</v>
       </c>
     </row>
     <row r="5">
@@ -842,13 +842,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.1321907583995</v>
+        <v>-0.1322</v>
       </c>
       <c r="C5" t="n">
-        <v>0.323816503312254</v>
+        <v>0.3238</v>
       </c>
       <c r="D5" t="n">
-        <v>0.683106758379441</v>
+        <v>0.6831</v>
       </c>
     </row>
     <row r="6">
@@ -856,13 +856,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.12105693994151</v>
+        <v>-1.1211</v>
       </c>
       <c r="C6" t="n">
-        <v>0.356033394513466</v>
+        <v>0.356</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00163975464278277</v>
+        <v>0.0016</v>
       </c>
     </row>
     <row r="7">
@@ -870,13 +870,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.377639777202835</v>
+        <v>0.3776</v>
       </c>
       <c r="C7" t="n">
-        <v>0.304016139312999</v>
+        <v>0.304</v>
       </c>
       <c r="D7" t="n">
-        <v>0.214173785886877</v>
+        <v>0.2142</v>
       </c>
     </row>
     <row r="8">
@@ -884,13 +884,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>0.821756402549003</v>
+        <v>0.8218</v>
       </c>
       <c r="C8" t="n">
-        <v>0.319701329503895</v>
+        <v>0.3197</v>
       </c>
       <c r="D8" t="n">
-        <v>0.010158472210531</v>
+        <v>0.0102</v>
       </c>
     </row>
     <row r="9">
@@ -898,13 +898,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.35849522573185</v>
+        <v>-1.3585</v>
       </c>
       <c r="C9" t="n">
-        <v>0.420233788296791</v>
+        <v>0.4202</v>
       </c>
       <c r="D9" t="n">
-        <v>0.00122620690118946</v>
+        <v>0.0012</v>
       </c>
     </row>
     <row r="10">
@@ -912,13 +912,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.861099148009334</v>
+        <v>-0.8611</v>
       </c>
       <c r="C10" t="n">
-        <v>0.324529533720654</v>
+        <v>0.3245</v>
       </c>
       <c r="D10" t="n">
-        <v>0.00796908469785711</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="11">
@@ -926,13 +926,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0387198775245461</v>
+        <v>-0.0387</v>
       </c>
       <c r="C11" t="n">
-        <v>0.325526911155548</v>
+        <v>0.3255</v>
       </c>
       <c r="D11" t="n">
-        <v>0.905318737498331</v>
+        <v>0.9053</v>
       </c>
     </row>
     <row r="12">
@@ -940,13 +940,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.564998778904266</v>
+        <v>-0.565</v>
       </c>
       <c r="C12" t="n">
-        <v>0.485716135157964</v>
+        <v>0.4857</v>
       </c>
       <c r="D12" t="n">
-        <v>0.244736866701062</v>
+        <v>0.2447</v>
       </c>
     </row>
     <row r="13">
@@ -954,13 +954,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.05729719321019</v>
+        <v>-1.0573</v>
       </c>
       <c r="C13" t="n">
-        <v>0.697494778217006</v>
+        <v>0.6975</v>
       </c>
       <c r="D13" t="n">
-        <v>0.129557382297949</v>
+        <v>0.1296</v>
       </c>
     </row>
     <row r="14">
@@ -968,13 +968,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.28542080199948</v>
+        <v>-1.2854</v>
       </c>
       <c r="C14" t="n">
-        <v>0.740278039169894</v>
+        <v>0.7403</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0824926513703027</v>
+        <v>0.0825</v>
       </c>
     </row>
     <row r="15">
@@ -982,13 +982,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.41578815361765</v>
+        <v>-1.4158</v>
       </c>
       <c r="C15" t="n">
-        <v>0.728684508681899</v>
+        <v>0.7287</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0520237607165542</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="16">
@@ -996,13 +996,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-1.30314677801982</v>
+        <v>-1.3031</v>
       </c>
       <c r="C16" t="n">
-        <v>0.698657237185131</v>
+        <v>0.6987</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0621511095168702</v>
+        <v>0.0622</v>
       </c>
     </row>
     <row r="17">
@@ -1010,13 +1010,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-1.09277975165252</v>
+        <v>-1.0928</v>
       </c>
       <c r="C17" t="n">
-        <v>0.672031993071463</v>
+        <v>0.672</v>
       </c>
       <c r="D17" t="n">
-        <v>0.103932015032744</v>
+        <v>0.1039</v>
       </c>
     </row>
     <row r="18">
@@ -1024,13 +1024,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-1.03818696892916</v>
+        <v>-1.0382</v>
       </c>
       <c r="C18" t="n">
-        <v>0.657653502071145</v>
+        <v>0.6577</v>
       </c>
       <c r="D18" t="n">
-        <v>0.114422547327424</v>
+        <v>0.1144</v>
       </c>
     </row>
     <row r="19">
@@ -1038,13 +1038,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-1.13035524651131</v>
+        <v>-1.1304</v>
       </c>
       <c r="C19" t="n">
-        <v>0.657506776848006</v>
+        <v>0.6575</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0855863782746068</v>
+        <v>0.0856</v>
       </c>
     </row>
     <row r="20">
@@ -1052,13 +1052,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.05174806831519</v>
+        <v>-1.0517</v>
       </c>
       <c r="C20" t="n">
-        <v>0.675630795008506</v>
+        <v>0.6756</v>
       </c>
       <c r="D20" t="n">
-        <v>0.119543975327657</v>
+        <v>0.1195</v>
       </c>
     </row>
     <row r="21">
@@ -1066,13 +1066,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.93456171186514</v>
+        <v>-0.9346</v>
       </c>
       <c r="C21" t="n">
-        <v>0.683281959505787</v>
+        <v>0.6833</v>
       </c>
       <c r="D21" t="n">
-        <v>0.171389054787642</v>
+        <v>0.1714</v>
       </c>
     </row>
     <row r="22">
@@ -1080,13 +1080,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-1.13360040303422</v>
+        <v>-1.1336</v>
       </c>
       <c r="C22" t="n">
-        <v>0.695163678473655</v>
+        <v>0.6952</v>
       </c>
       <c r="D22" t="n">
-        <v>0.102954549911525</v>
+        <v>0.103</v>
       </c>
     </row>
     <row r="23">
@@ -1094,13 +1094,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-1.4025892235245</v>
+        <v>-1.4026</v>
       </c>
       <c r="C23" t="n">
-        <v>0.87400605496044</v>
+        <v>0.874</v>
       </c>
       <c r="D23" t="n">
-        <v>0.108541778870265</v>
+        <v>0.1085</v>
       </c>
     </row>
     <row r="24">
@@ -1108,13 +1108,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.232917522181786</v>
+        <v>0.2329</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0549784234871216</v>
+        <v>0.055</v>
       </c>
       <c r="D24" t="n">
-        <v>0.000022700461552089</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1150,13 +1150,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.63985760396549</v>
+        <v>-1.6399</v>
       </c>
       <c r="C2" t="n">
-        <v>1.7119847068233</v>
+        <v>1.712</v>
       </c>
       <c r="D2" t="n">
-        <v>0.338128665494533</v>
+        <v>0.3381</v>
       </c>
     </row>
     <row r="3">
@@ -1164,13 +1164,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.119268163369971</v>
+        <v>-0.1193</v>
       </c>
       <c r="C3" t="n">
-        <v>0.336747928873695</v>
+        <v>0.3367</v>
       </c>
       <c r="D3" t="n">
-        <v>0.723206701711976</v>
+        <v>0.7232</v>
       </c>
     </row>
     <row r="4">
@@ -1178,13 +1178,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.178101232029074</v>
+        <v>-0.1781</v>
       </c>
       <c r="C4" t="n">
-        <v>0.364103154406656</v>
+        <v>0.3641</v>
       </c>
       <c r="D4" t="n">
-        <v>0.624735166663663</v>
+        <v>0.6247</v>
       </c>
     </row>
     <row r="5">
@@ -1192,13 +1192,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.22544325378988</v>
+        <v>-1.2254</v>
       </c>
       <c r="C5" t="n">
-        <v>0.69844192290108</v>
+        <v>0.6984</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0793382764903816</v>
+        <v>0.0793</v>
       </c>
     </row>
     <row r="6">
@@ -1206,13 +1206,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.102629469930867</v>
+        <v>-0.1026</v>
       </c>
       <c r="C6" t="n">
-        <v>1.10090224972129</v>
+        <v>1.1009</v>
       </c>
       <c r="D6" t="n">
-        <v>0.925726359654848</v>
+        <v>0.9257</v>
       </c>
     </row>
     <row r="7">
@@ -1220,13 +1220,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.42266763175141</v>
+        <v>0.4227</v>
       </c>
       <c r="C7" t="n">
-        <v>0.713752428241443</v>
+        <v>0.7138</v>
       </c>
       <c r="D7" t="n">
-        <v>0.553732200594692</v>
+        <v>0.5537</v>
       </c>
     </row>
     <row r="8">
@@ -1254,13 +1254,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.556340293043207</v>
+        <v>0.5563</v>
       </c>
       <c r="C10" t="n">
-        <v>0.736415560952545</v>
+        <v>0.7364</v>
       </c>
       <c r="D10" t="n">
-        <v>0.449966676533983</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="11">
@@ -1268,13 +1268,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.247554106150954</v>
+        <v>-0.2476</v>
       </c>
       <c r="C11" t="n">
-        <v>1.04768200033696</v>
+        <v>1.0477</v>
       </c>
       <c r="D11" t="n">
-        <v>0.813209626275475</v>
+        <v>0.8132</v>
       </c>
     </row>
     <row r="12">
@@ -1282,13 +1282,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0679442525922799</v>
+        <v>0.0679</v>
       </c>
       <c r="C12" t="n">
-        <v>1.05191018149522</v>
+        <v>1.0519</v>
       </c>
       <c r="D12" t="n">
-        <v>0.948499406930426</v>
+        <v>0.9485</v>
       </c>
     </row>
     <row r="13">
@@ -1296,13 +1296,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>0.143798307076691</v>
+        <v>0.1438</v>
       </c>
       <c r="C13" t="n">
-        <v>1.59378385483527</v>
+        <v>1.5938</v>
       </c>
       <c r="D13" t="n">
-        <v>0.928108837643466</v>
+        <v>0.9281</v>
       </c>
     </row>
     <row r="14">
@@ -1310,13 +1310,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>0.249830958106449</v>
+        <v>0.2498</v>
       </c>
       <c r="C14" t="n">
-        <v>1.7451710978706</v>
+        <v>1.7452</v>
       </c>
       <c r="D14" t="n">
-        <v>0.88616732066207</v>
+        <v>0.8862</v>
       </c>
     </row>
     <row r="15">
@@ -1324,13 +1324,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>0.369631336503031</v>
+        <v>0.3696</v>
       </c>
       <c r="C15" t="n">
-        <v>1.72149704582523</v>
+        <v>1.7215</v>
       </c>
       <c r="D15" t="n">
-        <v>0.829989482493843</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="16">
@@ -1338,13 +1338,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.468118911313132</v>
+        <v>0.4681</v>
       </c>
       <c r="C16" t="n">
-        <v>1.66711784833335</v>
+        <v>1.6671</v>
       </c>
       <c r="D16" t="n">
-        <v>0.778867383431452</v>
+        <v>0.7789</v>
       </c>
     </row>
     <row r="17">
@@ -1352,13 +1352,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.507487011531612</v>
+        <v>0.5075</v>
       </c>
       <c r="C17" t="n">
-        <v>1.61437219466819</v>
+        <v>1.6144</v>
       </c>
       <c r="D17" t="n">
-        <v>0.753250940428615</v>
+        <v>0.7533</v>
       </c>
     </row>
     <row r="18">
@@ -1366,13 +1366,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>0.484083843909326</v>
+        <v>0.4841</v>
       </c>
       <c r="C18" t="n">
-        <v>1.59680811921259</v>
+        <v>1.5968</v>
       </c>
       <c r="D18" t="n">
-        <v>0.761770080970127</v>
+        <v>0.7618</v>
       </c>
     </row>
     <row r="19">
@@ -1380,13 +1380,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>0.377353312920755</v>
+        <v>0.3774</v>
       </c>
       <c r="C19" t="n">
-        <v>1.59908776690256</v>
+        <v>1.5991</v>
       </c>
       <c r="D19" t="n">
-        <v>0.813447907373067</v>
+        <v>0.8134</v>
       </c>
     </row>
     <row r="20">
@@ -1394,13 +1394,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>0.221082067033935</v>
+        <v>0.2211</v>
       </c>
       <c r="C20" t="n">
-        <v>1.631638168552</v>
+        <v>1.6316</v>
       </c>
       <c r="D20" t="n">
-        <v>0.892218940830233</v>
+        <v>0.8922</v>
       </c>
     </row>
     <row r="21">
@@ -1408,13 +1408,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0864441601164589</v>
+        <v>0.0864</v>
       </c>
       <c r="C21" t="n">
-        <v>1.63848131917373</v>
+        <v>1.6385</v>
       </c>
       <c r="D21" t="n">
-        <v>0.957924160613751</v>
+        <v>0.9579</v>
       </c>
     </row>
     <row r="22">
@@ -1422,13 +1422,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.00510728173720448</v>
+        <v>0.0051</v>
       </c>
       <c r="C22" t="n">
-        <v>1.64115674043549</v>
+        <v>1.6412</v>
       </c>
       <c r="D22" t="n">
-        <v>0.997516986301226</v>
+        <v>0.9975</v>
       </c>
     </row>
     <row r="23">
@@ -1436,13 +1436,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.0627879417631931</v>
+        <v>-0.0628</v>
       </c>
       <c r="C23" t="n">
-        <v>1.94811596841063</v>
+        <v>1.9481</v>
       </c>
       <c r="D23" t="n">
-        <v>0.974288564885443</v>
+        <v>0.9743</v>
       </c>
     </row>
     <row r="24">
@@ -1450,7 +1450,7 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.54117999425717</v>
+        <v>0.5412</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -1492,13 +1492,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>2.80921671535414</v>
+        <v>2.8092</v>
       </c>
       <c r="C2" t="n">
-        <v>0.17971370267126</v>
+        <v>0.1797</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000443369840522243</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1506,13 +1506,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0311812545682837</v>
+        <v>0.0312</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0490708280547933</v>
+        <v>0.0491</v>
       </c>
       <c r="D3" t="n">
-        <v>0.525145638145358</v>
+        <v>0.5251</v>
       </c>
     </row>
     <row r="4">
@@ -1520,13 +1520,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0392402105844459</v>
+        <v>0.0392</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0460097081402118</v>
+        <v>0.046</v>
       </c>
       <c r="D4" t="n">
-        <v>0.393732475083097</v>
+        <v>0.3937</v>
       </c>
     </row>
     <row r="5">
@@ -1534,13 +1534,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.0530443618803046</v>
+        <v>-0.053</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0902600601625659</v>
+        <v>0.0903</v>
       </c>
       <c r="D5" t="n">
-        <v>0.556744649907599</v>
+        <v>0.5567</v>
       </c>
     </row>
     <row r="6">
@@ -1548,13 +1548,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0402986182974082</v>
+        <v>0.0403</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0823863715467429</v>
+        <v>0.0824</v>
       </c>
       <c r="D6" t="n">
-        <v>0.624741308096634</v>
+        <v>0.6247</v>
       </c>
     </row>
     <row r="7">
@@ -1562,13 +1562,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.137599147008558</v>
+        <v>-0.1376</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0857643887189523</v>
+        <v>0.0858</v>
       </c>
       <c r="D7" t="n">
-        <v>0.108629091472212</v>
+        <v>0.1086</v>
       </c>
     </row>
     <row r="8">
@@ -1576,13 +1576,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.0719631758589172</v>
+        <v>-0.072</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0931481340208779</v>
+        <v>0.0931</v>
       </c>
       <c r="D8" t="n">
-        <v>0.439778671870282</v>
+        <v>0.4398</v>
       </c>
     </row>
     <row r="9">
@@ -1590,13 +1590,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.178165127817341</v>
+        <v>-0.1782</v>
       </c>
       <c r="C9" t="n">
-        <v>0.104990486716803</v>
+        <v>0.105</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0897033740931516</v>
+        <v>0.0897</v>
       </c>
     </row>
     <row r="10">
@@ -1604,13 +1604,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.00382618498303945</v>
+        <v>0.0038</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0809810829033103</v>
+        <v>0.081</v>
       </c>
       <c r="D10" t="n">
-        <v>0.962315662505998</v>
+        <v>0.9623</v>
       </c>
     </row>
     <row r="11">
@@ -1618,13 +1618,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.116371816022432</v>
+        <v>-0.1164</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0933863872994384</v>
+        <v>0.0934</v>
       </c>
       <c r="D11" t="n">
-        <v>0.212715740220356</v>
+        <v>0.2127</v>
       </c>
     </row>
     <row r="12">
@@ -1632,13 +1632,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.0717851526046283</v>
+        <v>-0.0718</v>
       </c>
       <c r="C12" t="n">
-        <v>0.128340297560921</v>
+        <v>0.1283</v>
       </c>
       <c r="D12" t="n">
-        <v>0.575933473140579</v>
+        <v>0.5759</v>
       </c>
     </row>
     <row r="13">
@@ -1646,13 +1646,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.133660251290937</v>
+        <v>-0.1337</v>
       </c>
       <c r="C13" t="n">
-        <v>0.179610977150743</v>
+        <v>0.1796</v>
       </c>
       <c r="D13" t="n">
-        <v>0.45677649620694</v>
+        <v>0.4568</v>
       </c>
     </row>
     <row r="14">
@@ -1660,13 +1660,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.15030957941767</v>
+        <v>-0.1503</v>
       </c>
       <c r="C14" t="n">
-        <v>0.187033705783792</v>
+        <v>0.187</v>
       </c>
       <c r="D14" t="n">
-        <v>0.421599317918137</v>
+        <v>0.4216</v>
       </c>
     </row>
     <row r="15">
@@ -1674,13 +1674,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.17458224909525</v>
+        <v>-0.1746</v>
       </c>
       <c r="C15" t="n">
-        <v>0.183424234839812</v>
+        <v>0.1834</v>
       </c>
       <c r="D15" t="n">
-        <v>0.341201015010159</v>
+        <v>0.3412</v>
       </c>
     </row>
     <row r="16">
@@ -1688,13 +1688,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.220741946719498</v>
+        <v>-0.2207</v>
       </c>
       <c r="C16" t="n">
-        <v>0.175879982929213</v>
+        <v>0.1759</v>
       </c>
       <c r="D16" t="n">
-        <v>0.209452820384383</v>
+        <v>0.2095</v>
       </c>
     </row>
     <row r="17">
@@ -1702,13 +1702,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.247196309050597</v>
+        <v>-0.2472</v>
       </c>
       <c r="C17" t="n">
-        <v>0.170779236598456</v>
+        <v>0.1708</v>
       </c>
       <c r="D17" t="n">
-        <v>0.147767811700006</v>
+        <v>0.1478</v>
       </c>
     </row>
     <row r="18">
@@ -1716,13 +1716,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.233535084545207</v>
+        <v>-0.2335</v>
       </c>
       <c r="C18" t="n">
-        <v>0.167087630976878</v>
+        <v>0.1671</v>
       </c>
       <c r="D18" t="n">
-        <v>0.162209102777322</v>
+        <v>0.1622</v>
       </c>
     </row>
     <row r="19">
@@ -1730,13 +1730,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.199407339193454</v>
+        <v>-0.1994</v>
       </c>
       <c r="C19" t="n">
-        <v>0.166605134964734</v>
+        <v>0.1666</v>
       </c>
       <c r="D19" t="n">
-        <v>0.231351025308984</v>
+        <v>0.2314</v>
       </c>
     </row>
     <row r="20">
@@ -1744,13 +1744,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.195575636546001</v>
+        <v>-0.1956</v>
       </c>
       <c r="C20" t="n">
-        <v>0.17327044805438</v>
+        <v>0.1733</v>
       </c>
       <c r="D20" t="n">
-        <v>0.259011545939185</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="21">
@@ -1758,13 +1758,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.205999822162982</v>
+        <v>-0.206</v>
       </c>
       <c r="C21" t="n">
-        <v>0.177325960331365</v>
+        <v>0.1773</v>
       </c>
       <c r="D21" t="n">
-        <v>0.245356763577084</v>
+        <v>0.2454</v>
       </c>
     </row>
     <row r="22">
@@ -1772,13 +1772,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.174246659552308</v>
+        <v>-0.1742</v>
       </c>
       <c r="C22" t="n">
-        <v>0.181883022830822</v>
+        <v>0.1819</v>
       </c>
       <c r="D22" t="n">
-        <v>0.33805520744544</v>
+        <v>0.3381</v>
       </c>
     </row>
     <row r="23">
@@ -1786,13 +1786,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.130172041649697</v>
+        <v>-0.1302</v>
       </c>
       <c r="C23" t="n">
-        <v>0.234320638206979</v>
+        <v>0.2343</v>
       </c>
       <c r="D23" t="n">
-        <v>0.578532495223294</v>
+        <v>0.5785</v>
       </c>
     </row>
     <row r="24">
@@ -1800,13 +1800,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.50924124144369</v>
+        <v>-1.5092</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0795660774058807</v>
+        <v>0.0796</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000311231882259371</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1842,13 +1842,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.0942210348075</v>
+        <v>3.0942</v>
       </c>
       <c r="C2" t="n">
-        <v>0.374278601057852</v>
+        <v>0.3743</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000000000000000137187930526539</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1856,13 +1856,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.0018233624772592</v>
+        <v>-0.0018</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0958362360129506</v>
+        <v>0.0958</v>
       </c>
       <c r="D3" t="n">
-        <v>0.984820511904647</v>
+        <v>0.9848</v>
       </c>
     </row>
     <row r="4">
@@ -1870,13 +1870,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.000884055833716306</v>
+        <v>-0.0009</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0900396542386214</v>
+        <v>0.09</v>
       </c>
       <c r="D4" t="n">
-        <v>0.992166083118184</v>
+        <v>0.9922</v>
       </c>
     </row>
     <row r="5">
@@ -1884,13 +1884,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.00168418118929125</v>
+        <v>0.0017</v>
       </c>
       <c r="C5" t="n">
-        <v>0.18722871366248</v>
+        <v>0.1872</v>
       </c>
       <c r="D5" t="n">
-        <v>0.992822874118568</v>
+        <v>0.9928</v>
       </c>
     </row>
     <row r="6">
@@ -1898,13 +1898,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.179948245896301</v>
+        <v>0.1799</v>
       </c>
       <c r="C6" t="n">
-        <v>0.186679542470245</v>
+        <v>0.1867</v>
       </c>
       <c r="D6" t="n">
-        <v>0.335075020443712</v>
+        <v>0.3351</v>
       </c>
     </row>
     <row r="7">
@@ -1912,13 +1912,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.313591601023681</v>
+        <v>-0.3136</v>
       </c>
       <c r="C7" t="n">
-        <v>0.18349091225726</v>
+        <v>0.1835</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0874452641308215</v>
+        <v>0.0874</v>
       </c>
     </row>
     <row r="8">
@@ -1926,13 +1926,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.171476049410045</v>
+        <v>-0.1715</v>
       </c>
       <c r="C8" t="n">
-        <v>0.204153038738045</v>
+        <v>0.2042</v>
       </c>
       <c r="D8" t="n">
-        <v>0.40094272610526</v>
+        <v>0.4009</v>
       </c>
     </row>
     <row r="9">
@@ -1940,13 +1940,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0584331618589349</v>
+        <v>0.0584</v>
       </c>
       <c r="C9" t="n">
-        <v>0.218043606032045</v>
+        <v>0.218</v>
       </c>
       <c r="D9" t="n">
-        <v>0.78870823096141</v>
+        <v>0.7887</v>
       </c>
     </row>
     <row r="10">
@@ -1954,13 +1954,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.395004633748591</v>
+        <v>0.395</v>
       </c>
       <c r="C10" t="n">
-        <v>0.17039983116384</v>
+        <v>0.1704</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0204436365692366</v>
+        <v>0.0204</v>
       </c>
     </row>
     <row r="11">
@@ -1968,13 +1968,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0789423134082052</v>
+        <v>-0.0789</v>
       </c>
       <c r="C11" t="n">
-        <v>0.195759283366634</v>
+        <v>0.1958</v>
       </c>
       <c r="D11" t="n">
-        <v>0.686755368363364</v>
+        <v>0.6868</v>
       </c>
     </row>
     <row r="12">
@@ -1982,13 +1982,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.323188701534309</v>
+        <v>-0.3232</v>
       </c>
       <c r="C12" t="n">
-        <v>0.266760143374256</v>
+        <v>0.2668</v>
       </c>
       <c r="D12" t="n">
-        <v>0.225691217014766</v>
+        <v>0.2257</v>
       </c>
     </row>
     <row r="13">
@@ -1996,13 +1996,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.613236545029909</v>
+        <v>-0.6132</v>
       </c>
       <c r="C13" t="n">
-        <v>0.374045116129475</v>
+        <v>0.374</v>
       </c>
       <c r="D13" t="n">
-        <v>0.101114969365379</v>
+        <v>0.1011</v>
       </c>
     </row>
     <row r="14">
@@ -2010,13 +2010,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.688493638434468</v>
+        <v>-0.6885</v>
       </c>
       <c r="C14" t="n">
-        <v>0.392585109734575</v>
+        <v>0.3926</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0794744446092783</v>
+        <v>0.0795</v>
       </c>
     </row>
     <row r="15">
@@ -2024,13 +2024,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.584239368799399</v>
+        <v>-0.5842</v>
       </c>
       <c r="C15" t="n">
-        <v>0.383659419522862</v>
+        <v>0.3837</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1278069204593</v>
+        <v>0.1278</v>
       </c>
     </row>
     <row r="16">
@@ -2038,13 +2038,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.472078083046865</v>
+        <v>-0.4721</v>
       </c>
       <c r="C16" t="n">
-        <v>0.362257271919948</v>
+        <v>0.3623</v>
       </c>
       <c r="D16" t="n">
-        <v>0.192521182694599</v>
+        <v>0.1925</v>
       </c>
     </row>
     <row r="17">
@@ -2052,13 +2052,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.377150049585725</v>
+        <v>-0.3772</v>
       </c>
       <c r="C17" t="n">
-        <v>0.34857958331942</v>
+        <v>0.3486</v>
       </c>
       <c r="D17" t="n">
-        <v>0.279269175720271</v>
+        <v>0.2793</v>
       </c>
     </row>
     <row r="18">
@@ -2066,13 +2066,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.341141072721015</v>
+        <v>-0.3411</v>
       </c>
       <c r="C18" t="n">
-        <v>0.342756922556087</v>
+        <v>0.3428</v>
       </c>
       <c r="D18" t="n">
-        <v>0.319597317780357</v>
+        <v>0.3196</v>
       </c>
     </row>
     <row r="19">
@@ -2080,13 +2080,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.371409432904821</v>
+        <v>-0.3714</v>
       </c>
       <c r="C19" t="n">
-        <v>0.342501725314751</v>
+        <v>0.3425</v>
       </c>
       <c r="D19" t="n">
-        <v>0.278186756556359</v>
+        <v>0.2782</v>
       </c>
     </row>
     <row r="20">
@@ -2094,13 +2094,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.423721884485117</v>
+        <v>-0.4237</v>
       </c>
       <c r="C20" t="n">
-        <v>0.358940738430898</v>
+        <v>0.3589</v>
       </c>
       <c r="D20" t="n">
-        <v>0.237809890191846</v>
+        <v>0.2378</v>
       </c>
     </row>
     <row r="21">
@@ -2108,13 +2108,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.465170008006705</v>
+        <v>-0.4652</v>
       </c>
       <c r="C21" t="n">
-        <v>0.371703588638339</v>
+        <v>0.3717</v>
       </c>
       <c r="D21" t="n">
-        <v>0.210768822413617</v>
+        <v>0.2108</v>
       </c>
     </row>
     <row r="22">
@@ -2122,13 +2122,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.51025058521999</v>
+        <v>-0.5103</v>
       </c>
       <c r="C22" t="n">
-        <v>0.388498067555917</v>
+        <v>0.3885</v>
       </c>
       <c r="D22" t="n">
-        <v>0.189050604650804</v>
+        <v>0.1891</v>
       </c>
     </row>
     <row r="23">
@@ -2136,13 +2136,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.564670607661701</v>
+        <v>-0.5647</v>
       </c>
       <c r="C23" t="n">
-        <v>0.506301873102446</v>
+        <v>0.5063</v>
       </c>
       <c r="D23" t="n">
-        <v>0.264728545492681</v>
+        <v>0.2647</v>
       </c>
     </row>
     <row r="24">
@@ -2150,13 +2150,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.845226728084796</v>
+        <v>-0.8452</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0784253825954999</v>
+        <v>0.0784</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00000000000000000000000000439845636742376</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2192,13 +2192,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>1.2969057781922</v>
+        <v>1.2969</v>
       </c>
       <c r="C2" t="n">
-        <v>0.301976620366303</v>
+        <v>0.302</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000017491200275895</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2206,13 +2206,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.358299583071426</v>
+        <v>-0.3583</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0817359408466906</v>
+        <v>0.0817</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0000116721481454232</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2220,13 +2220,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.446931567738043</v>
+        <v>-0.4469</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0836292150471837</v>
+        <v>0.0836</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0000000908153523362293</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2234,13 +2234,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.280407229496759</v>
+        <v>-0.2804</v>
       </c>
       <c r="C5" t="n">
-        <v>0.180269665044719</v>
+        <v>0.1803</v>
       </c>
       <c r="D5" t="n">
-        <v>0.119829984378295</v>
+        <v>0.1198</v>
       </c>
     </row>
     <row r="6">
@@ -2248,13 +2248,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.83268591652951</v>
+        <v>0.8327</v>
       </c>
       <c r="C6" t="n">
-        <v>0.158404954630576</v>
+        <v>0.1584</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00000014667035339377</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2262,13 +2262,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.255770064964641</v>
+        <v>0.2558</v>
       </c>
       <c r="C7" t="n">
-        <v>0.149635907652562</v>
+        <v>0.1496</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0873986003550043</v>
+        <v>0.0874</v>
       </c>
     </row>
     <row r="8">
@@ -2276,13 +2276,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.03090488684111</v>
+        <v>-1.0309</v>
       </c>
       <c r="C8" t="n">
-        <v>0.201040535432247</v>
+        <v>0.201</v>
       </c>
       <c r="D8" t="n">
-        <v>0.000000293076163738361</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2290,13 +2290,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.704448297634375</v>
+        <v>0.7044</v>
       </c>
       <c r="C9" t="n">
-        <v>0.179504804511613</v>
+        <v>0.1795</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0000869468847603924</v>
+        <v>0.0001</v>
       </c>
     </row>
     <row r="10">
@@ -2304,13 +2304,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.602560533319542</v>
+        <v>0.6026</v>
       </c>
       <c r="C10" t="n">
-        <v>0.155945647351354</v>
+        <v>0.1559</v>
       </c>
       <c r="D10" t="n">
-        <v>0.000111584628811875</v>
+        <v>0.0001</v>
       </c>
     </row>
     <row r="11">
@@ -2318,13 +2318,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0585492487112331</v>
+        <v>-0.0585</v>
       </c>
       <c r="C11" t="n">
-        <v>0.20959025422241</v>
+        <v>0.2096</v>
       </c>
       <c r="D11" t="n">
-        <v>0.779975465192125</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="12">
@@ -2332,13 +2332,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0269242355406962</v>
+        <v>0.0269</v>
       </c>
       <c r="C12" t="n">
-        <v>0.207330862653963</v>
+        <v>0.2073</v>
       </c>
       <c r="D12" t="n">
-        <v>0.896676238685559</v>
+        <v>0.8967</v>
       </c>
     </row>
     <row r="13">
@@ -2346,13 +2346,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>0.052308310572871</v>
+        <v>0.0523</v>
       </c>
       <c r="C13" t="n">
-        <v>0.289020898077135</v>
+        <v>0.289</v>
       </c>
       <c r="D13" t="n">
-        <v>0.85637972100604</v>
+        <v>0.8564</v>
       </c>
     </row>
     <row r="14">
@@ -2360,13 +2360,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0778760728399267</v>
+        <v>0.0779</v>
       </c>
       <c r="C14" t="n">
-        <v>0.30112299363397</v>
+        <v>0.3011</v>
       </c>
       <c r="D14" t="n">
-        <v>0.795929362037257</v>
+        <v>0.7959</v>
       </c>
     </row>
     <row r="15">
@@ -2374,13 +2374,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0991995481238758</v>
+        <v>0.0992</v>
       </c>
       <c r="C15" t="n">
-        <v>0.295164560658492</v>
+        <v>0.2952</v>
       </c>
       <c r="D15" t="n">
-        <v>0.736808898202418</v>
+        <v>0.7368</v>
       </c>
     </row>
     <row r="16">
@@ -2388,13 +2388,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0602266881069433</v>
+        <v>0.0602</v>
       </c>
       <c r="C16" t="n">
-        <v>0.282782391858891</v>
+        <v>0.2828</v>
       </c>
       <c r="D16" t="n">
-        <v>0.831343405725632</v>
+        <v>0.8313</v>
       </c>
     </row>
     <row r="17">
@@ -2402,13 +2402,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0191399367893719</v>
+        <v>0.0191</v>
       </c>
       <c r="C17" t="n">
-        <v>0.27656870770341</v>
+        <v>0.2766</v>
       </c>
       <c r="D17" t="n">
-        <v>0.944826445032952</v>
+        <v>0.9448</v>
       </c>
     </row>
     <row r="18">
@@ -2416,13 +2416,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.0500879153338468</v>
+        <v>-0.0501</v>
       </c>
       <c r="C18" t="n">
-        <v>0.273721297366712</v>
+        <v>0.2737</v>
       </c>
       <c r="D18" t="n">
-        <v>0.854806853573217</v>
+        <v>0.8548</v>
       </c>
     </row>
     <row r="19">
@@ -2430,13 +2430,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.11586269795559</v>
+        <v>-0.1159</v>
       </c>
       <c r="C19" t="n">
-        <v>0.272998437927959</v>
+        <v>0.273</v>
       </c>
       <c r="D19" t="n">
-        <v>0.67126834905191</v>
+        <v>0.6713</v>
       </c>
     </row>
     <row r="20">
@@ -2444,13 +2444,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.0912120596425448</v>
+        <v>-0.0912</v>
       </c>
       <c r="C20" t="n">
-        <v>0.284289075261788</v>
+        <v>0.2843</v>
       </c>
       <c r="D20" t="n">
-        <v>0.748329638279143</v>
+        <v>0.7483</v>
       </c>
     </row>
     <row r="21">
@@ -2458,13 +2458,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0396405836665468</v>
+        <v>0.0396</v>
       </c>
       <c r="C21" t="n">
-        <v>0.289731962166835</v>
+        <v>0.2897</v>
       </c>
       <c r="D21" t="n">
-        <v>0.891174557100648</v>
+        <v>0.8912</v>
       </c>
     </row>
     <row r="22">
@@ -2472,13 +2472,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.186404419725476</v>
+        <v>0.1864</v>
       </c>
       <c r="C22" t="n">
-        <v>0.29404053812076</v>
+        <v>0.294</v>
       </c>
       <c r="D22" t="n">
-        <v>0.526119178466631</v>
+        <v>0.5261</v>
       </c>
     </row>
     <row r="23">
@@ -2486,13 +2486,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>0.335308635618812</v>
+        <v>0.3353</v>
       </c>
       <c r="C23" t="n">
-        <v>0.378533932614072</v>
+        <v>0.3785</v>
       </c>
       <c r="D23" t="n">
-        <v>0.37572064245356</v>
+        <v>0.3757</v>
       </c>
     </row>
     <row r="24">
@@ -2500,13 +2500,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.738426191743074</v>
+        <v>-0.7384</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0537767234145931</v>
+        <v>0.0538</v>
       </c>
       <c r="D24" t="n">
-        <v>0.000000000000000000000000000000000000000000659080114814377</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2542,13 +2542,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.25402503775698</v>
+        <v>3.254</v>
       </c>
       <c r="C2" t="n">
-        <v>2.13881401084254</v>
+        <v>2.1388</v>
       </c>
       <c r="D2" t="n">
-        <v>0.128155572292059</v>
+        <v>0.1282</v>
       </c>
     </row>
     <row r="3">
@@ -2556,13 +2556,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.53907634076338</v>
+        <v>1.5391</v>
       </c>
       <c r="C3" t="n">
-        <v>0.574731256408406</v>
+        <v>0.5747</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00740839828488199</v>
+        <v>0.0074</v>
       </c>
     </row>
     <row r="4">
@@ -2570,13 +2570,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.710125630822808</v>
+        <v>0.7101</v>
       </c>
       <c r="C4" t="n">
-        <v>0.547540426182637</v>
+        <v>0.5475</v>
       </c>
       <c r="D4" t="n">
-        <v>0.194652743043003</v>
+        <v>0.1947</v>
       </c>
     </row>
     <row r="5">
@@ -2584,13 +2584,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.923979976331419</v>
+        <v>0.924</v>
       </c>
       <c r="C5" t="n">
-        <v>0.703277924798839</v>
+        <v>0.7033</v>
       </c>
       <c r="D5" t="n">
-        <v>0.188907085510505</v>
+        <v>0.1889</v>
       </c>
     </row>
     <row r="6">
@@ -2598,13 +2598,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.01127397393401</v>
+        <v>-1.0113</v>
       </c>
       <c r="C6" t="n">
-        <v>0.932337078422503</v>
+        <v>0.9323</v>
       </c>
       <c r="D6" t="n">
-        <v>0.27806978074295</v>
+        <v>0.2781</v>
       </c>
     </row>
     <row r="7">
@@ -2612,13 +2612,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-5.23716093251764</v>
+        <v>-5.2372</v>
       </c>
       <c r="C7" t="n">
-        <v>12.4554408663258</v>
+        <v>12.4554</v>
       </c>
       <c r="D7" t="n">
-        <v>0.674140867534233</v>
+        <v>0.6741</v>
       </c>
     </row>
     <row r="8">
@@ -2626,13 +2626,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>1.45725880003159</v>
+        <v>1.4573</v>
       </c>
       <c r="C8" t="n">
-        <v>0.63528096155391</v>
+        <v>0.6353</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0217973465847249</v>
+        <v>0.0218</v>
       </c>
     </row>
     <row r="9">
@@ -2640,13 +2640,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.72274911916047</v>
+        <v>-1.7227</v>
       </c>
       <c r="C9" t="n">
-        <v>1.33523999513731</v>
+        <v>1.3352</v>
       </c>
       <c r="D9" t="n">
-        <v>0.19697538288805</v>
+        <v>0.197</v>
       </c>
     </row>
     <row r="10">
@@ -2654,13 +2654,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.384527599158822</v>
+        <v>-0.3845</v>
       </c>
       <c r="C10" t="n">
-        <v>1.02540886924046</v>
+        <v>1.0254</v>
       </c>
       <c r="D10" t="n">
-        <v>0.707660993793897</v>
+        <v>0.7077</v>
       </c>
     </row>
     <row r="11">
@@ -2668,13 +2668,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-5.20407102590059</v>
+        <v>-5.2041</v>
       </c>
       <c r="C11" t="n">
-        <v>40.5621218446947</v>
+        <v>40.5621</v>
       </c>
       <c r="D11" t="n">
-        <v>0.897912525103192</v>
+        <v>0.8979</v>
       </c>
     </row>
     <row r="12">
@@ -2682,13 +2682,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-3.18362628089906</v>
+        <v>-3.1836</v>
       </c>
       <c r="C12" t="n">
-        <v>1.54801078167911</v>
+        <v>1.548</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0397255076041237</v>
+        <v>0.0397</v>
       </c>
     </row>
     <row r="13">
@@ -2696,13 +2696,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-5.93043878459935</v>
+        <v>-5.9304</v>
       </c>
       <c r="C13" t="n">
-        <v>2.24558990895221</v>
+        <v>2.2456</v>
       </c>
       <c r="D13" t="n">
-        <v>0.00826795577584686</v>
+        <v>0.0083</v>
       </c>
     </row>
     <row r="14">
@@ -2710,13 +2710,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-7.09382529525264</v>
+        <v>-7.0938</v>
       </c>
       <c r="C14" t="n">
-        <v>2.49752648275794</v>
+        <v>2.4975</v>
       </c>
       <c r="D14" t="n">
-        <v>0.00450654211861647</v>
+        <v>0.0045</v>
       </c>
     </row>
     <row r="15">
@@ -2724,13 +2724,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-6.9859325494539</v>
+        <v>-6.9859</v>
       </c>
       <c r="C15" t="n">
-        <v>2.50476169523193</v>
+        <v>2.5048</v>
       </c>
       <c r="D15" t="n">
-        <v>0.00528611472540033</v>
+        <v>0.0053</v>
       </c>
     </row>
     <row r="16">
@@ -2738,13 +2738,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-6.32193424020449</v>
+        <v>-6.3219</v>
       </c>
       <c r="C16" t="n">
-        <v>2.3375280494704</v>
+        <v>2.3375</v>
       </c>
       <c r="D16" t="n">
-        <v>0.00683993750772423</v>
+        <v>0.0068</v>
       </c>
     </row>
     <row r="17">
@@ -2752,13 +2752,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-5.88091794014399</v>
+        <v>-5.8809</v>
       </c>
       <c r="C17" t="n">
-        <v>2.15031821097157</v>
+        <v>2.1503</v>
       </c>
       <c r="D17" t="n">
-        <v>0.00623981130848142</v>
+        <v>0.0062</v>
       </c>
     </row>
     <row r="18">
@@ -2766,13 +2766,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-5.7223695222892</v>
+        <v>-5.7224</v>
       </c>
       <c r="C18" t="n">
-        <v>2.04890879544729</v>
+        <v>2.0489</v>
       </c>
       <c r="D18" t="n">
-        <v>0.00522400332781252</v>
+        <v>0.0052</v>
       </c>
     </row>
     <row r="19">
@@ -2780,13 +2780,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-5.3076533241389</v>
+        <v>-5.3077</v>
       </c>
       <c r="C19" t="n">
-        <v>2.04641909185465</v>
+        <v>2.0464</v>
       </c>
       <c r="D19" t="n">
-        <v>0.00949687127309367</v>
+        <v>0.0095</v>
       </c>
     </row>
     <row r="20">
@@ -2794,13 +2794,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-5.04379259407137</v>
+        <v>-5.0438</v>
       </c>
       <c r="C20" t="n">
-        <v>2.11539561305439</v>
+        <v>2.1154</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0171104410393367</v>
+        <v>0.0171</v>
       </c>
     </row>
     <row r="21">
@@ -2808,13 +2808,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-4.80431512712981</v>
+        <v>-4.8043</v>
       </c>
       <c r="C21" t="n">
-        <v>2.16726859787823</v>
+        <v>2.1673</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0266394713259504</v>
+        <v>0.0266</v>
       </c>
     </row>
     <row r="22">
@@ -2822,13 +2822,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-4.4976754222135</v>
+        <v>-4.4977</v>
       </c>
       <c r="C22" t="n">
-        <v>2.19374627134785</v>
+        <v>2.1937</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0403423917403379</v>
+        <v>0.0403</v>
       </c>
     </row>
     <row r="23">
@@ -2836,13 +2836,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-4.22020817142323</v>
+        <v>-4.2202</v>
       </c>
       <c r="C23" t="n">
-        <v>2.66924305710593</v>
+        <v>2.6692</v>
       </c>
       <c r="D23" t="n">
-        <v>0.113866482793387</v>
+        <v>0.1139</v>
       </c>
     </row>
     <row r="24">
@@ -2850,13 +2850,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.300710509927211</v>
+        <v>0.3007</v>
       </c>
       <c r="C24" t="n">
-        <v>0.16640196290246</v>
+        <v>0.1664</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0707415148980519</v>
+        <v>0.0707</v>
       </c>
     </row>
   </sheetData>
@@ -2892,13 +2892,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.22939812473685</v>
+        <v>3.2294</v>
       </c>
       <c r="C2" t="n">
-        <v>0.523033890351718</v>
+        <v>0.523</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000000000664331471450255</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2906,13 +2906,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.0638985704384752</v>
+        <v>-0.0639</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1525947434978</v>
+        <v>0.1526</v>
       </c>
       <c r="D3" t="n">
-        <v>0.67540114136511</v>
+        <v>0.6754</v>
       </c>
     </row>
     <row r="4">
@@ -2920,13 +2920,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.221256414812613</v>
+        <v>0.2213</v>
       </c>
       <c r="C4" t="n">
-        <v>0.132666309798706</v>
+        <v>0.1327</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0953621069566502</v>
+        <v>0.0954</v>
       </c>
     </row>
     <row r="5">
@@ -2934,13 +2934,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.137340352397815</v>
+        <v>-0.1373</v>
       </c>
       <c r="C5" t="n">
-        <v>0.244044088156356</v>
+        <v>0.244</v>
       </c>
       <c r="D5" t="n">
-        <v>0.573592457377822</v>
+        <v>0.5736</v>
       </c>
     </row>
     <row r="6">
@@ -2948,13 +2948,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0174368985549959</v>
+        <v>0.0174</v>
       </c>
       <c r="C6" t="n">
-        <v>0.247853395914897</v>
+        <v>0.2479</v>
       </c>
       <c r="D6" t="n">
-        <v>0.943913763296226</v>
+        <v>0.9439</v>
       </c>
     </row>
     <row r="7">
@@ -2962,13 +2962,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.858778922268932</v>
+        <v>-0.8588</v>
       </c>
       <c r="C7" t="n">
-        <v>0.269043644917213</v>
+        <v>0.269</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00141306592054011</v>
+        <v>0.0014</v>
       </c>
     </row>
     <row r="8">
@@ -2976,13 +2976,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.257408277671643</v>
+        <v>-0.2574</v>
       </c>
       <c r="C8" t="n">
-        <v>0.260883956197871</v>
+        <v>0.2609</v>
       </c>
       <c r="D8" t="n">
-        <v>0.323800861469911</v>
+        <v>0.3238</v>
       </c>
     </row>
     <row r="9">
@@ -2990,13 +2990,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.371325972008166</v>
+        <v>-0.3713</v>
       </c>
       <c r="C9" t="n">
-        <v>0.304837669082233</v>
+        <v>0.3048</v>
       </c>
       <c r="D9" t="n">
-        <v>0.223181976176494</v>
+        <v>0.2232</v>
       </c>
     </row>
     <row r="10">
@@ -3004,13 +3004,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.0462645658198621</v>
+        <v>-0.0463</v>
       </c>
       <c r="C10" t="n">
-        <v>0.243426232462401</v>
+        <v>0.2434</v>
       </c>
       <c r="D10" t="n">
-        <v>0.849265410146681</v>
+        <v>0.8493</v>
       </c>
     </row>
     <row r="11">
@@ -3018,13 +3018,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.171009871089868</v>
+        <v>0.171</v>
       </c>
       <c r="C11" t="n">
-        <v>0.245563184507662</v>
+        <v>0.2456</v>
       </c>
       <c r="D11" t="n">
-        <v>0.486179205939902</v>
+        <v>0.4862</v>
       </c>
     </row>
     <row r="12">
@@ -3032,13 +3032,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.198676997716067</v>
+        <v>-0.1987</v>
       </c>
       <c r="C12" t="n">
-        <v>0.368507173783138</v>
+        <v>0.3685</v>
       </c>
       <c r="D12" t="n">
-        <v>0.589790182085035</v>
+        <v>0.5898</v>
       </c>
     </row>
     <row r="13">
@@ -3046,13 +3046,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.350918870736727</v>
+        <v>-0.3509</v>
       </c>
       <c r="C13" t="n">
-        <v>0.521377959944596</v>
+        <v>0.5214</v>
       </c>
       <c r="D13" t="n">
-        <v>0.500908850534131</v>
+        <v>0.5009</v>
       </c>
     </row>
     <row r="14">
@@ -3060,13 +3060,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.304066838978776</v>
+        <v>-0.3041</v>
       </c>
       <c r="C14" t="n">
-        <v>0.546306609784913</v>
+        <v>0.5463</v>
       </c>
       <c r="D14" t="n">
-        <v>0.577810035701122</v>
+        <v>0.5778</v>
       </c>
     </row>
     <row r="15">
@@ -3074,13 +3074,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.272922754796057</v>
+        <v>-0.2729</v>
       </c>
       <c r="C15" t="n">
-        <v>0.536366643946169</v>
+        <v>0.5364</v>
       </c>
       <c r="D15" t="n">
-        <v>0.610867056224194</v>
+        <v>0.6109</v>
       </c>
     </row>
     <row r="16">
@@ -3088,13 +3088,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.375491921131798</v>
+        <v>-0.3755</v>
       </c>
       <c r="C16" t="n">
-        <v>0.515627434549903</v>
+        <v>0.5156</v>
       </c>
       <c r="D16" t="n">
-        <v>0.466476894161327</v>
+        <v>0.4665</v>
       </c>
     </row>
     <row r="17">
@@ -3102,13 +3102,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.495709830448953</v>
+        <v>-0.4957</v>
       </c>
       <c r="C17" t="n">
-        <v>0.50128125221702</v>
+        <v>0.5013</v>
       </c>
       <c r="D17" t="n">
-        <v>0.322719098565502</v>
+        <v>0.3227</v>
       </c>
     </row>
     <row r="18">
@@ -3116,13 +3116,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.565269396398953</v>
+        <v>-0.5653</v>
       </c>
       <c r="C18" t="n">
-        <v>0.493227601880066</v>
+        <v>0.4932</v>
       </c>
       <c r="D18" t="n">
-        <v>0.251769512316663</v>
+        <v>0.2518</v>
       </c>
     </row>
     <row r="19">
@@ -3130,13 +3130,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.577648809669089</v>
+        <v>-0.5776</v>
       </c>
       <c r="C19" t="n">
-        <v>0.494047436676341</v>
+        <v>0.494</v>
       </c>
       <c r="D19" t="n">
-        <v>0.242316093012056</v>
+        <v>0.2423</v>
       </c>
     </row>
     <row r="20">
@@ -3144,13 +3144,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.602742422552697</v>
+        <v>-0.6027</v>
       </c>
       <c r="C20" t="n">
-        <v>0.512761223830128</v>
+        <v>0.5128</v>
       </c>
       <c r="D20" t="n">
-        <v>0.239801284299003</v>
+        <v>0.2398</v>
       </c>
     </row>
     <row r="21">
@@ -3158,13 +3158,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.479381137064827</v>
+        <v>-0.4794</v>
       </c>
       <c r="C21" t="n">
-        <v>0.523945871270541</v>
+        <v>0.5239</v>
       </c>
       <c r="D21" t="n">
-        <v>0.360221023670381</v>
+        <v>0.3602</v>
       </c>
     </row>
     <row r="22">
@@ -3172,13 +3172,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.247493274973949</v>
+        <v>-0.2475</v>
       </c>
       <c r="C22" t="n">
-        <v>0.543108616563125</v>
+        <v>0.5431</v>
       </c>
       <c r="D22" t="n">
-        <v>0.648607472078708</v>
+        <v>0.6486</v>
       </c>
     </row>
     <row r="23">
@@ -3186,13 +3186,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.0137880033876967</v>
+        <v>-0.0138</v>
       </c>
       <c r="C23" t="n">
-        <v>0.695838130213171</v>
+        <v>0.6958</v>
       </c>
       <c r="D23" t="n">
-        <v>0.984190985396012</v>
+        <v>0.9842</v>
       </c>
     </row>
     <row r="24">
@@ -3200,13 +3200,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.235736282944101</v>
+        <v>-0.2357</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0734220473422019</v>
+        <v>0.0734</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00132411365598545</v>
+        <v>0.0013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update results with full uncertainty about the non-detects
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -450,13 +450,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-3.8498</v>
+        <v>2.0747</v>
       </c>
       <c r="C2" t="n">
-        <v>1.3138</v>
+        <v>1.5514</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0034</v>
+        <v>0.1811</v>
       </c>
     </row>
     <row r="3">
@@ -464,13 +464,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.4534</v>
+        <v>-0.406</v>
       </c>
       <c r="C3" t="n">
-        <v>0.461</v>
+        <v>1.5495</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3254</v>
+        <v>0.7933</v>
       </c>
     </row>
     <row r="4">
@@ -478,13 +478,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.0764</v>
+        <v>-0.3068</v>
       </c>
       <c r="C4" t="n">
-        <v>0.364</v>
+        <v>0.5054</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8336</v>
+        <v>0.5438</v>
       </c>
     </row>
     <row r="5">
@@ -492,10 +492,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>4.9721</v>
+        <v>0.9294</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3255</v>
+        <v>0.2186</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -536,13 +536,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>4.8168</v>
+        <v>0.2639</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5349</v>
+        <v>3.2132</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.9345</v>
       </c>
     </row>
     <row r="10">
@@ -570,13 +570,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.8109</v>
+        <v>-0.8483</v>
       </c>
       <c r="C12" t="n">
-        <v>1.2127</v>
+        <v>1.6522</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5037</v>
+        <v>0.6077</v>
       </c>
     </row>
     <row r="13">
@@ -584,13 +584,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.3786</v>
+        <v>-1.5957</v>
       </c>
       <c r="C13" t="n">
-        <v>1.6571</v>
+        <v>2.153</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4054</v>
+        <v>0.4586</v>
       </c>
     </row>
     <row r="14">
@@ -598,13 +598,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.1254</v>
+        <v>-1.9388</v>
       </c>
       <c r="C14" t="n">
-        <v>1.6482</v>
+        <v>2.4238</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4947</v>
+        <v>0.4238</v>
       </c>
     </row>
     <row r="15">
@@ -612,13 +612,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.5373</v>
+        <v>-1.926</v>
       </c>
       <c r="C15" t="n">
-        <v>1.5159</v>
+        <v>2.3084</v>
       </c>
       <c r="D15" t="n">
-        <v>0.723</v>
+        <v>0.4041</v>
       </c>
     </row>
     <row r="16">
@@ -626,13 +626,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.2627</v>
+        <v>-1.6234</v>
       </c>
       <c r="C16" t="n">
-        <v>1.4354</v>
+        <v>1.908</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8548</v>
+        <v>0.3949</v>
       </c>
     </row>
     <row r="17">
@@ -640,13 +640,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.0795</v>
+        <v>-1.0878</v>
       </c>
       <c r="C17" t="n">
-        <v>1.3691</v>
+        <v>1.6023</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9537</v>
+        <v>0.4972</v>
       </c>
     </row>
     <row r="18">
@@ -654,13 +654,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.0175</v>
+        <v>-0.9956</v>
       </c>
       <c r="C18" t="n">
-        <v>1.3388</v>
+        <v>1.5973</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9895</v>
+        <v>0.5331</v>
       </c>
     </row>
     <row r="19">
@@ -668,13 +668,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.3573</v>
+        <v>-1.4435</v>
       </c>
       <c r="C19" t="n">
-        <v>1.3415</v>
+        <v>1.5876</v>
       </c>
       <c r="D19" t="n">
-        <v>0.79</v>
+        <v>0.3632</v>
       </c>
     </row>
     <row r="20">
@@ -682,13 +682,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.4158</v>
+        <v>-1.4987</v>
       </c>
       <c r="C20" t="n">
-        <v>1.4431</v>
+        <v>1.9321</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7732</v>
+        <v>0.4379</v>
       </c>
     </row>
     <row r="21">
@@ -696,13 +696,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.1843</v>
+        <v>-1.5555</v>
       </c>
       <c r="C21" t="n">
-        <v>1.5328</v>
+        <v>3.3057</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9043</v>
+        <v>0.638</v>
       </c>
     </row>
     <row r="22">
@@ -710,13 +710,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1104</v>
+        <v>-1.6126</v>
       </c>
       <c r="C22" t="n">
-        <v>1.9673</v>
+        <v>5.4767</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9552</v>
+        <v>0.7684</v>
       </c>
     </row>
     <row r="23">
@@ -724,13 +724,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>0.4052</v>
+        <v>-1.6697</v>
       </c>
       <c r="C23" t="n">
-        <v>3.017</v>
+        <v>8.2019</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8932</v>
+        <v>0.8387</v>
       </c>
     </row>
     <row r="24">
@@ -738,13 +738,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.44</v>
+        <v>-1.8861</v>
       </c>
       <c r="C24" t="n">
-        <v>0.2188</v>
+        <v>0.4379</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0443</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -780,13 +780,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>2.1137</v>
+        <v>2.6353</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8564</v>
+        <v>0.3605</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0136</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -794,13 +794,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1951</v>
+        <v>0.1302</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2229</v>
+        <v>0.0924</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3814</v>
+        <v>0.1586</v>
       </c>
     </row>
     <row r="4">
@@ -808,13 +808,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.071</v>
+        <v>0.0416</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2078</v>
+        <v>0.0871</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7325</v>
+        <v>0.6332</v>
       </c>
     </row>
     <row r="5">
@@ -822,13 +822,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.3394</v>
+        <v>0.2237</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3939</v>
+        <v>0.1549</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3889</v>
+        <v>0.1486</v>
       </c>
     </row>
     <row r="6">
@@ -836,13 +836,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.26</v>
+        <v>-0.5301</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4286</v>
+        <v>0.2023</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0033</v>
+        <v>0.0088</v>
       </c>
     </row>
     <row r="7">
@@ -850,13 +850,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.3888</v>
+        <v>0.241</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3683</v>
+        <v>0.147</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2912</v>
+        <v>0.1011</v>
       </c>
     </row>
     <row r="8">
@@ -864,13 +864,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8245</v>
+        <v>0.3141</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3888</v>
+        <v>0.1548</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0339</v>
+        <v>0.0424</v>
       </c>
     </row>
     <row r="9">
@@ -878,13 +878,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.6249</v>
+        <v>-0.3997</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5088</v>
+        <v>0.2154</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0014</v>
+        <v>0.0634</v>
       </c>
     </row>
     <row r="10">
@@ -892,13 +892,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.0262</v>
+        <v>-0.2778</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3934</v>
+        <v>0.1692</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0091</v>
+        <v>0.1006</v>
       </c>
     </row>
     <row r="11">
@@ -906,13 +906,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1129</v>
+        <v>-0.1211</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3969</v>
+        <v>0.1674</v>
       </c>
       <c r="D11" t="n">
-        <v>0.776</v>
+        <v>0.4696</v>
       </c>
     </row>
     <row r="12">
@@ -920,13 +920,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.6174</v>
+        <v>-0.2446</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5979</v>
+        <v>0.2505</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3018</v>
+        <v>0.3288</v>
       </c>
     </row>
     <row r="13">
@@ -934,13 +934,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.1661</v>
+        <v>-0.4456</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8552</v>
+        <v>0.3584</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1728</v>
+        <v>0.2137</v>
       </c>
     </row>
     <row r="14">
@@ -948,13 +948,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.412</v>
+        <v>-0.5311</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9051</v>
+        <v>0.3789</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1187</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="15">
@@ -962,13 +962,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.5311</v>
+        <v>-0.5908</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8902</v>
+        <v>0.3746</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0855</v>
+        <v>0.1148</v>
       </c>
     </row>
     <row r="16">
@@ -976,13 +976,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-1.3716</v>
+        <v>-0.5513</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8535</v>
+        <v>0.3624</v>
       </c>
       <c r="D16" t="n">
-        <v>0.108</v>
+        <v>0.1282</v>
       </c>
     </row>
     <row r="17">
@@ -990,13 +990,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-1.0943</v>
+        <v>-0.4823</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8221</v>
+        <v>0.3485</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1832</v>
+        <v>0.1664</v>
       </c>
     </row>
     <row r="18">
@@ -1004,13 +1004,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-1.021</v>
+        <v>-0.4713</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8052</v>
+        <v>0.3404</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2048</v>
+        <v>0.1661</v>
       </c>
     </row>
     <row r="19">
@@ -1018,13 +1018,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-1.1421</v>
+        <v>-0.5076</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8049</v>
+        <v>0.3404</v>
       </c>
       <c r="D19" t="n">
-        <v>0.156</v>
+        <v>0.1359</v>
       </c>
     </row>
     <row r="20">
@@ -1032,13 +1032,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.0763</v>
+        <v>-0.4477</v>
       </c>
       <c r="C20" t="n">
-        <v>0.8272</v>
+        <v>0.3486</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1932</v>
+        <v>0.1991</v>
       </c>
     </row>
     <row r="21">
@@ -1046,13 +1046,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.9681</v>
+        <v>-0.3903</v>
       </c>
       <c r="C21" t="n">
-        <v>0.8368</v>
+        <v>0.3512</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2473</v>
+        <v>0.2663</v>
       </c>
     </row>
     <row r="22">
@@ -1060,13 +1060,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-1.2366</v>
+        <v>-0.555</v>
       </c>
       <c r="C22" t="n">
-        <v>0.8502</v>
+        <v>0.3548</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1458</v>
+        <v>0.1178</v>
       </c>
     </row>
     <row r="23">
@@ -1074,13 +1074,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-1.5875</v>
+        <v>-0.7725</v>
       </c>
       <c r="C23" t="n">
-        <v>1.0697</v>
+        <v>0.4429</v>
       </c>
       <c r="D23" t="n">
-        <v>0.1378</v>
+        <v>0.0811</v>
       </c>
     </row>
     <row r="24">
@@ -1088,10 +1088,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.4245</v>
+        <v>-0.6532</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0579</v>
+        <v>0.0589</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -1130,13 +1130,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.7155</v>
+        <v>0.6536</v>
       </c>
       <c r="C2" t="n">
-        <v>1.7419</v>
+        <v>1.1937</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3247</v>
+        <v>0.584</v>
       </c>
     </row>
     <row r="3">
@@ -1144,13 +1144,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.1578</v>
+        <v>-0.2104</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3368</v>
+        <v>0.28</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6393</v>
+        <v>0.4523</v>
       </c>
     </row>
     <row r="4">
@@ -1158,13 +1158,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.2295</v>
+        <v>-0.1423</v>
       </c>
       <c r="C4" t="n">
-        <v>0.365</v>
+        <v>0.2809</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5294</v>
+        <v>0.6125</v>
       </c>
     </row>
     <row r="5">
@@ -1172,13 +1172,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.8713</v>
+        <v>-4.1308</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7077</v>
+        <v>31132.3064</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0082</v>
+        <v>0.9999</v>
       </c>
     </row>
     <row r="6">
@@ -1186,13 +1186,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.1283</v>
+        <v>-0.1033</v>
       </c>
       <c r="C6" t="n">
-        <v>1.1042</v>
+        <v>0.5976</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9075</v>
+        <v>0.8627</v>
       </c>
     </row>
     <row r="7">
@@ -1200,47 +1200,55 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.5193</v>
+        <v>0.3199</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7278</v>
+        <v>0.4924</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4755</v>
+        <v>0.516</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" t="n">
+        <v>-4.2098</v>
+      </c>
       <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8"/>
+        <v>33127.983</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.9999</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9"/>
+      <c r="B9" t="n">
+        <v>-3.3352</v>
+      </c>
       <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9"/>
+        <v>34711.4847</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.9999</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6714</v>
+        <v>0.7964</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7539</v>
+        <v>0.4608</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3731</v>
+        <v>0.0839</v>
       </c>
     </row>
     <row r="11">
@@ -1248,13 +1256,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.2992</v>
+        <v>-0.3848</v>
       </c>
       <c r="C11" t="n">
-        <v>1.044</v>
+        <v>0.6546</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7744</v>
+        <v>0.5567</v>
       </c>
     </row>
     <row r="12">
@@ -1262,13 +1270,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0885</v>
+        <v>-0.1796</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0604</v>
+        <v>0.8383</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9335</v>
+        <v>0.8304</v>
       </c>
     </row>
     <row r="13">
@@ -1276,13 +1284,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>0.186</v>
+        <v>-0.3215</v>
       </c>
       <c r="C13" t="n">
-        <v>1.6111</v>
+        <v>1.2172</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9081</v>
+        <v>0.7917</v>
       </c>
     </row>
     <row r="14">
@@ -1290,13 +1298,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>0.3173</v>
+        <v>-0.2983</v>
       </c>
       <c r="C14" t="n">
-        <v>1.7675</v>
+        <v>1.2949</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8575</v>
+        <v>0.8178</v>
       </c>
     </row>
     <row r="15">
@@ -1304,13 +1312,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>0.4642</v>
+        <v>-0.0764</v>
       </c>
       <c r="C15" t="n">
-        <v>1.7446</v>
+        <v>1.2655</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7902</v>
+        <v>0.9519</v>
       </c>
     </row>
     <row r="16">
@@ -1318,13 +1326,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.5861</v>
+        <v>0.2627</v>
       </c>
       <c r="C16" t="n">
-        <v>1.6932</v>
+        <v>1.183</v>
       </c>
       <c r="D16" t="n">
-        <v>0.7292</v>
+        <v>0.8242</v>
       </c>
     </row>
     <row r="17">
@@ -1332,13 +1340,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.638</v>
+        <v>0.6006</v>
       </c>
       <c r="C17" t="n">
-        <v>1.6422</v>
+        <v>1.1302</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6977</v>
+        <v>0.5952</v>
       </c>
     </row>
     <row r="18">
@@ -1346,13 +1354,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>0.6114</v>
+        <v>0.797</v>
       </c>
       <c r="C18" t="n">
-        <v>1.6252</v>
+        <v>1.1185</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7068</v>
+        <v>0.4761</v>
       </c>
     </row>
     <row r="19">
@@ -1360,13 +1368,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>0.4813</v>
+        <v>0.3992</v>
       </c>
       <c r="C19" t="n">
-        <v>1.6278</v>
+        <v>1.119</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7675</v>
+        <v>0.7213</v>
       </c>
     </row>
     <row r="20">
@@ -1374,13 +1382,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>0.2986</v>
+        <v>0.0343</v>
       </c>
       <c r="C20" t="n">
-        <v>1.6597</v>
+        <v>1.1592</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8572</v>
+        <v>0.9764</v>
       </c>
     </row>
     <row r="21">
@@ -1388,13 +1396,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1468</v>
+        <v>0.0067</v>
       </c>
       <c r="C21" t="n">
-        <v>1.6654</v>
+        <v>1.1774</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9298</v>
+        <v>0.9955</v>
       </c>
     </row>
     <row r="22">
@@ -1402,13 +1410,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0626</v>
+        <v>0.2032</v>
       </c>
       <c r="C22" t="n">
-        <v>1.6704</v>
+        <v>1.1655</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9701</v>
+        <v>0.8616</v>
       </c>
     </row>
     <row r="23">
@@ -1416,13 +1424,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.0046</v>
+        <v>0.4415</v>
       </c>
       <c r="C23" t="n">
-        <v>1.9816</v>
+        <v>1.4466</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9982</v>
+        <v>0.7602</v>
       </c>
     </row>
     <row r="24">
@@ -1430,13 +1438,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.5273</v>
+        <v>-0.2729</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>0.1272</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>0.032</v>
       </c>
     </row>
   </sheetData>
@@ -1472,10 +1480,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>2.8092</v>
+        <v>2.8062</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1797</v>
+        <v>0.1794</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1486,13 +1494,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0312</v>
+        <v>0.0303</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0491</v>
+        <v>0.049</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5251</v>
+        <v>0.5363</v>
       </c>
     </row>
     <row r="4">
@@ -1500,13 +1508,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0392</v>
+        <v>0.0409</v>
       </c>
       <c r="C4" t="n">
-        <v>0.046</v>
+        <v>0.0459</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3937</v>
+        <v>0.3729</v>
       </c>
     </row>
     <row r="5">
@@ -1514,13 +1522,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.053</v>
+        <v>-0.0508</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0903</v>
+        <v>0.09</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5567</v>
+        <v>0.5723</v>
       </c>
     </row>
     <row r="6">
@@ -1528,13 +1536,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0403</v>
+        <v>0.0425</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0824</v>
+        <v>0.0822</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6247</v>
+        <v>0.6055</v>
       </c>
     </row>
     <row r="7">
@@ -1542,13 +1550,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.1376</v>
+        <v>-0.1305</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0858</v>
+        <v>0.0857</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1086</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="8">
@@ -1556,13 +1564,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.072</v>
+        <v>-0.0705</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0931</v>
+        <v>0.0929</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4398</v>
+        <v>0.448</v>
       </c>
     </row>
     <row r="9">
@@ -1570,13 +1578,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.1782</v>
+        <v>-0.1751</v>
       </c>
       <c r="C9" t="n">
-        <v>0.105</v>
+        <v>0.1048</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0897</v>
+        <v>0.0948</v>
       </c>
     </row>
     <row r="10">
@@ -1584,13 +1592,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0038</v>
+        <v>0.0062</v>
       </c>
       <c r="C10" t="n">
-        <v>0.081</v>
+        <v>0.0808</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9623</v>
+        <v>0.9385</v>
       </c>
     </row>
     <row r="11">
@@ -1598,13 +1606,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.1164</v>
+        <v>-0.1154</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0934</v>
+        <v>0.0932</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2127</v>
+        <v>0.2155</v>
       </c>
     </row>
     <row r="12">
@@ -1612,13 +1620,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.0718</v>
+        <v>-0.0717</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1283</v>
+        <v>0.1281</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5759</v>
+        <v>0.5758</v>
       </c>
     </row>
     <row r="13">
@@ -1626,13 +1634,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.1337</v>
+        <v>-0.1335</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1796</v>
+        <v>0.1793</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4568</v>
+        <v>0.4565</v>
       </c>
     </row>
     <row r="14">
@@ -1640,10 +1648,10 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.1503</v>
+        <v>-0.15</v>
       </c>
       <c r="C14" t="n">
-        <v>0.187</v>
+        <v>0.1866</v>
       </c>
       <c r="D14" t="n">
         <v>0.4216</v>
@@ -1654,13 +1662,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.1746</v>
+        <v>-0.1739</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1834</v>
+        <v>0.183</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3412</v>
+        <v>0.3419</v>
       </c>
     </row>
     <row r="16">
@@ -1668,13 +1676,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.2207</v>
+        <v>-0.2197</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1759</v>
+        <v>0.1755</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2095</v>
+        <v>0.2106</v>
       </c>
     </row>
     <row r="17">
@@ -1682,13 +1690,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.2472</v>
+        <v>-0.2461</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1708</v>
+        <v>0.1704</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1478</v>
+        <v>0.1487</v>
       </c>
     </row>
     <row r="18">
@@ -1696,13 +1704,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.2335</v>
+        <v>-0.2325</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1671</v>
+        <v>0.1667</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1622</v>
+        <v>0.1632</v>
       </c>
     </row>
     <row r="19">
@@ -1710,13 +1718,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.1994</v>
+        <v>-0.1979</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1666</v>
+        <v>0.1663</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2314</v>
+        <v>0.234</v>
       </c>
     </row>
     <row r="20">
@@ -1724,13 +1732,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.1956</v>
+        <v>-0.1916</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1733</v>
+        <v>0.1729</v>
       </c>
       <c r="D20" t="n">
-        <v>0.259</v>
+        <v>0.2678</v>
       </c>
     </row>
     <row r="21">
@@ -1738,13 +1746,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.206</v>
+        <v>-0.2</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1773</v>
+        <v>0.177</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2454</v>
+        <v>0.2585</v>
       </c>
     </row>
     <row r="22">
@@ -1752,13 +1760,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.1742</v>
+        <v>-0.1708</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1819</v>
+        <v>0.1814</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3381</v>
+        <v>0.3462</v>
       </c>
     </row>
     <row r="23">
@@ -1766,13 +1774,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.1302</v>
+        <v>-0.1306</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2343</v>
+        <v>0.2335</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5785</v>
+        <v>0.5759</v>
       </c>
     </row>
     <row r="24">
@@ -1780,10 +1788,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.5092</v>
+        <v>-1.5118</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0796</v>
+        <v>0.0797</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -1822,10 +1830,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.0942</v>
+        <v>3.6956</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3743</v>
+        <v>0.5517</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1836,13 +1844,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.0018</v>
+        <v>0.0617</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0958</v>
+        <v>0.0931</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9848</v>
+        <v>0.5074</v>
       </c>
     </row>
     <row r="4">
@@ -1850,13 +1858,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.0009</v>
+        <v>-0.0038</v>
       </c>
       <c r="C4" t="n">
-        <v>0.09</v>
+        <v>0.0992</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9922</v>
+        <v>0.9695</v>
       </c>
     </row>
     <row r="5">
@@ -1864,13 +1872,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0017</v>
+        <v>0.2732</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1872</v>
+        <v>0.4071</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9928</v>
+        <v>0.5022</v>
       </c>
     </row>
     <row r="6">
@@ -1878,13 +1886,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1799</v>
+        <v>0.3417</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1867</v>
+        <v>0.4097</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3351</v>
+        <v>0.4043</v>
       </c>
     </row>
     <row r="7">
@@ -1892,13 +1900,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.3136</v>
+        <v>0.0394</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1835</v>
+        <v>0.4375</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0874</v>
+        <v>0.9282</v>
       </c>
     </row>
     <row r="8">
@@ -1906,13 +1914,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.1715</v>
+        <v>-0.0368</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2042</v>
+        <v>0.508</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4009</v>
+        <v>0.9422</v>
       </c>
     </row>
     <row r="9">
@@ -1920,13 +1928,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0584</v>
+        <v>0.0543</v>
       </c>
       <c r="C9" t="n">
-        <v>0.218</v>
+        <v>0.467</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7887</v>
+        <v>0.9074</v>
       </c>
     </row>
     <row r="10">
@@ -1934,13 +1942,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.395</v>
+        <v>0.5066</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1704</v>
+        <v>0.4029</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0204</v>
+        <v>0.2086</v>
       </c>
     </row>
     <row r="11">
@@ -1948,13 +1956,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0789</v>
+        <v>0.2517</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1958</v>
+        <v>0.407</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6868</v>
+        <v>0.5363</v>
       </c>
     </row>
     <row r="12">
@@ -1962,13 +1970,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.3232</v>
+        <v>-0.3645</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2668</v>
+        <v>0.3331</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2257</v>
+        <v>0.2739</v>
       </c>
     </row>
     <row r="13">
@@ -1976,13 +1984,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.6132</v>
+        <v>-0.6841</v>
       </c>
       <c r="C13" t="n">
-        <v>0.374</v>
+        <v>0.4614</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1011</v>
+        <v>0.1382</v>
       </c>
     </row>
     <row r="14">
@@ -1990,13 +1998,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.6885</v>
+        <v>-0.7966</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3926</v>
+        <v>0.4828</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0795</v>
+        <v>0.0989</v>
       </c>
     </row>
     <row r="15">
@@ -2004,13 +2012,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.5842</v>
+        <v>-0.7271</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3837</v>
+        <v>0.461</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1278</v>
+        <v>0.1147</v>
       </c>
     </row>
     <row r="16">
@@ -2018,13 +2026,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.4721</v>
+        <v>-0.5878</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3623</v>
+        <v>0.4163</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1925</v>
+        <v>0.158</v>
       </c>
     </row>
     <row r="17">
@@ -2032,13 +2040,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.3772</v>
+        <v>-0.4762</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3486</v>
+        <v>0.3919</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2793</v>
+        <v>0.2243</v>
       </c>
     </row>
     <row r="18">
@@ -2046,13 +2054,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.3411</v>
+        <v>-0.4278</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3428</v>
+        <v>0.3856</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3196</v>
+        <v>0.2673</v>
       </c>
     </row>
     <row r="19">
@@ -2060,13 +2068,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.3714</v>
+        <v>-0.4209</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3425</v>
+        <v>0.3858</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2782</v>
+        <v>0.2753</v>
       </c>
     </row>
     <row r="20">
@@ -2074,13 +2082,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.4237</v>
+        <v>-0.4618</v>
       </c>
       <c r="C20" t="n">
-        <v>0.3589</v>
+        <v>0.4089</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2378</v>
+        <v>0.2587</v>
       </c>
     </row>
     <row r="21">
@@ -2088,13 +2096,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.4652</v>
+        <v>-0.5497</v>
       </c>
       <c r="C21" t="n">
-        <v>0.3717</v>
+        <v>0.4485</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2108</v>
+        <v>0.2203</v>
       </c>
     </row>
     <row r="22">
@@ -2102,13 +2110,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.5103</v>
+        <v>-0.6302</v>
       </c>
       <c r="C22" t="n">
-        <v>0.3885</v>
+        <v>0.5566</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1891</v>
+        <v>0.2575</v>
       </c>
     </row>
     <row r="23">
@@ -2116,13 +2124,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.5647</v>
+        <v>-0.7091</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5063</v>
+        <v>0.8097</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2647</v>
+        <v>0.3812</v>
       </c>
     </row>
     <row r="24">
@@ -2130,10 +2138,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.8452</v>
+        <v>-1.2996</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0784</v>
+        <v>0.1361</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -2172,10 +2180,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>1.2916</v>
+        <v>2.5842</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3039</v>
+        <v>0.4867</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2186,13 +2194,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.3517</v>
+        <v>-0.2709</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0822</v>
+        <v>0.1375</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.0489</v>
       </c>
     </row>
     <row r="4">
@@ -2200,13 +2208,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.4499</v>
+        <v>-0.3324</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0842</v>
+        <v>0.1702</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.0509</v>
       </c>
     </row>
     <row r="5">
@@ -2214,13 +2222,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.2822</v>
+        <v>-0.3055</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1812</v>
+        <v>0.6103</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1195</v>
+        <v>0.6167</v>
       </c>
     </row>
     <row r="6">
@@ -2228,13 +2236,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.836</v>
+        <v>0.1735</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1593</v>
+        <v>0.3265</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.595</v>
       </c>
     </row>
     <row r="7">
@@ -2242,13 +2250,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2685</v>
+        <v>0.0735</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1506</v>
+        <v>0.3305</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0747</v>
+        <v>0.8241</v>
       </c>
     </row>
     <row r="8">
@@ -2256,13 +2264,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.0291</v>
+        <v>-0.4025</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2023</v>
+        <v>0.9186</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.6612</v>
       </c>
     </row>
     <row r="9">
@@ -2270,13 +2278,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7086</v>
+        <v>0.3616</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1806</v>
+        <v>0.3416</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0001</v>
+        <v>0.2899</v>
       </c>
     </row>
     <row r="10">
@@ -2284,13 +2292,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6053</v>
+        <v>0.2979</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1569</v>
+        <v>0.3143</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0001</v>
+        <v>0.3432</v>
       </c>
     </row>
     <row r="11">
@@ -2298,13 +2306,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0603</v>
+        <v>-0.5077</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2103</v>
+        <v>2.6812</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7743</v>
+        <v>0.8498</v>
       </c>
     </row>
     <row r="12">
@@ -2312,13 +2320,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0262</v>
+        <v>-0.0752</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2088</v>
+        <v>0.3127</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9003</v>
+        <v>0.8099</v>
       </c>
     </row>
     <row r="13">
@@ -2326,13 +2334,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0508</v>
+        <v>-0.1424</v>
       </c>
       <c r="C13" t="n">
-        <v>0.291</v>
+        <v>0.422</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8614</v>
+        <v>0.7358</v>
       </c>
     </row>
     <row r="14">
@@ -2340,13 +2348,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0763</v>
+        <v>-0.1519</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3031</v>
+        <v>0.4318</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8013</v>
+        <v>0.7251</v>
       </c>
     </row>
     <row r="15">
@@ -2354,13 +2362,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0979</v>
+        <v>-0.0794</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2971</v>
+        <v>0.4257</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7418</v>
+        <v>0.852</v>
       </c>
     </row>
     <row r="16">
@@ -2368,13 +2376,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.059</v>
+        <v>0.0283</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2847</v>
+        <v>0.4025</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8357</v>
+        <v>0.944</v>
       </c>
     </row>
     <row r="17">
@@ -2382,13 +2390,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0178</v>
+        <v>0.1148</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2784</v>
+        <v>0.3913</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9492</v>
+        <v>0.7693</v>
       </c>
     </row>
     <row r="18">
@@ -2396,13 +2404,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.0503</v>
+        <v>0.0939</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2755</v>
+        <v>0.3884</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8551</v>
+        <v>0.809</v>
       </c>
     </row>
     <row r="19">
@@ -2410,13 +2418,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.1113</v>
+        <v>-0.0478</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2748</v>
+        <v>0.3883</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6855</v>
+        <v>0.902</v>
       </c>
     </row>
     <row r="20">
@@ -2424,13 +2432,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.082</v>
+        <v>-0.103</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2862</v>
+        <v>0.4176</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7745</v>
+        <v>0.8051</v>
       </c>
     </row>
     <row r="21">
@@ -2438,13 +2446,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0486</v>
+        <v>-0.0682</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2917</v>
+        <v>0.4417</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8676</v>
+        <v>0.8773</v>
       </c>
     </row>
     <row r="22">
@@ -2452,13 +2460,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1852</v>
+        <v>0.015</v>
       </c>
       <c r="C22" t="n">
-        <v>0.296</v>
+        <v>0.4708</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5314</v>
+        <v>0.9746</v>
       </c>
     </row>
     <row r="23">
@@ -2466,13 +2474,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>0.3216</v>
+        <v>0.1064</v>
       </c>
       <c r="C23" t="n">
-        <v>0.381</v>
+        <v>0.6381</v>
       </c>
       <c r="D23" t="n">
-        <v>0.3987</v>
+        <v>0.8676</v>
       </c>
     </row>
     <row r="24">
@@ -2480,10 +2488,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.7311</v>
+        <v>-1.3911</v>
       </c>
       <c r="C24" t="n">
-        <v>0.054</v>
+        <v>0.1179</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -2522,13 +2530,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.256</v>
+        <v>3.5343</v>
       </c>
       <c r="C2" t="n">
-        <v>2.3514</v>
+        <v>800.2282</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1661</v>
+        <v>0.9965</v>
       </c>
     </row>
     <row r="3">
@@ -2536,13 +2544,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.6934</v>
+        <v>0.583</v>
       </c>
       <c r="C3" t="n">
-        <v>0.633</v>
+        <v>0.6629</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0075</v>
+        <v>0.3791</v>
       </c>
     </row>
     <row r="4">
@@ -2550,13 +2558,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.7922</v>
+        <v>0.4571</v>
       </c>
       <c r="C4" t="n">
-        <v>0.605</v>
+        <v>0.6524</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1904</v>
+        <v>0.4835</v>
       </c>
     </row>
     <row r="5">
@@ -2564,13 +2572,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0925</v>
+        <v>0.9492</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7798</v>
+        <v>800.2225</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1612</v>
+        <v>0.9991</v>
       </c>
     </row>
     <row r="6">
@@ -2578,13 +2586,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.0716</v>
+        <v>-0.3583</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0438</v>
+        <v>800.2244</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3046</v>
+        <v>0.9996</v>
       </c>
     </row>
     <row r="7">
@@ -2592,13 +2600,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-4.9626</v>
+        <v>-1.1288</v>
       </c>
       <c r="C7" t="n">
-        <v>6.4371</v>
+        <v>32520.1465</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4407</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -2606,13 +2614,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>1.6365</v>
+        <v>0.8908</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7045</v>
+        <v>800.2225</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0202</v>
+        <v>0.9991</v>
       </c>
     </row>
     <row r="9">
@@ -2620,13 +2628,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.6899</v>
+        <v>-0.4345</v>
       </c>
       <c r="C9" t="n">
-        <v>1.4738</v>
+        <v>800.2271</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2515</v>
+        <v>0.9996</v>
       </c>
     </row>
     <row r="10">
@@ -2634,13 +2642,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.4317</v>
+        <v>0.235</v>
       </c>
       <c r="C10" t="n">
-        <v>1.1469</v>
+        <v>800.2257</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7066</v>
+        <v>0.9998</v>
       </c>
     </row>
     <row r="11">
@@ -2648,13 +2656,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-4.785</v>
+        <v>-0.2914</v>
       </c>
       <c r="C11" t="n">
-        <v>15.6994</v>
+        <v>46626.5467</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7605</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -2662,13 +2670,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-3.38</v>
+        <v>-1.0657</v>
       </c>
       <c r="C12" t="n">
-        <v>1.6877</v>
+        <v>1.4366</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0452</v>
+        <v>0.4582</v>
       </c>
     </row>
     <row r="13">
@@ -2676,13 +2684,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-6.289</v>
+        <v>-2.0273</v>
       </c>
       <c r="C13" t="n">
-        <v>2.4502</v>
+        <v>2.2512</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0103</v>
+        <v>0.3678</v>
       </c>
     </row>
     <row r="14">
@@ -2690,13 +2698,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-7.505</v>
+        <v>-2.6432</v>
       </c>
       <c r="C14" t="n">
-        <v>2.7197</v>
+        <v>2.7724</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0058</v>
+        <v>0.3404</v>
       </c>
     </row>
     <row r="15">
@@ -2704,13 +2712,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-7.3581</v>
+        <v>-2.9255</v>
       </c>
       <c r="C15" t="n">
-        <v>2.7257</v>
+        <v>3.0265</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0069</v>
+        <v>0.3337</v>
       </c>
     </row>
     <row r="16">
@@ -2718,13 +2726,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-6.6172</v>
+        <v>-2.9003</v>
       </c>
       <c r="C16" t="n">
-        <v>2.5527</v>
+        <v>3.0756</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0095</v>
+        <v>0.3457</v>
       </c>
     </row>
     <row r="17">
@@ -2732,13 +2740,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-6.1393</v>
+        <v>-2.5941</v>
       </c>
       <c r="C17" t="n">
-        <v>2.3587</v>
+        <v>3.0473</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0092</v>
+        <v>0.3946</v>
       </c>
     </row>
     <row r="18">
@@ -2746,13 +2754,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-6.0682</v>
+        <v>-2.0346</v>
       </c>
       <c r="C18" t="n">
-        <v>2.2502</v>
+        <v>3.0463</v>
       </c>
       <c r="D18" t="n">
-        <v>0.007</v>
+        <v>0.5042</v>
       </c>
     </row>
     <row r="19">
@@ -2760,13 +2768,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-5.7058</v>
+        <v>-2.1229</v>
       </c>
       <c r="C19" t="n">
-        <v>2.2482</v>
+        <v>3.0302</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0111</v>
+        <v>0.4836</v>
       </c>
     </row>
     <row r="20">
@@ -2774,13 +2782,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-5.3884</v>
+        <v>-2.2595</v>
       </c>
       <c r="C20" t="n">
-        <v>2.3214</v>
+        <v>3.0375</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0203</v>
+        <v>0.457</v>
       </c>
     </row>
     <row r="21">
@@ -2788,13 +2796,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-5.0532</v>
+        <v>-2.0468</v>
       </c>
       <c r="C21" t="n">
-        <v>2.3757</v>
+        <v>3.0412</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0334</v>
+        <v>0.5009</v>
       </c>
     </row>
     <row r="22">
@@ -2802,13 +2810,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-4.664</v>
+        <v>-2.227</v>
       </c>
       <c r="C22" t="n">
-        <v>2.4047</v>
+        <v>3.0786</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0524</v>
+        <v>0.4695</v>
       </c>
     </row>
     <row r="23">
@@ -2816,13 +2824,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-4.3204</v>
+        <v>-2.4611</v>
       </c>
       <c r="C23" t="n">
-        <v>2.9231</v>
+        <v>3.3358</v>
       </c>
       <c r="D23" t="n">
-        <v>0.1394</v>
+        <v>0.4606</v>
       </c>
     </row>
     <row r="24">
@@ -2830,13 +2838,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.4191</v>
+        <v>-1.5916</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1689</v>
+        <v>0.3486</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0131</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2872,10 +2880,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.2298</v>
+        <v>3.27</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5242</v>
+        <v>0.5094</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2886,13 +2894,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.0653</v>
+        <v>-0.0697</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1529</v>
+        <v>0.1491</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6693</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="4">
@@ -2900,13 +2908,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2206</v>
+        <v>0.2093</v>
       </c>
       <c r="C4" t="n">
-        <v>0.133</v>
+        <v>0.1289</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0971</v>
+        <v>0.1044</v>
       </c>
     </row>
     <row r="5">
@@ -2914,13 +2922,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.1363</v>
+        <v>-0.1329</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2446</v>
+        <v>0.2392</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5774</v>
+        <v>0.5783</v>
       </c>
     </row>
     <row r="6">
@@ -2928,13 +2936,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0175</v>
+        <v>0.0402</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2484</v>
+        <v>0.2417</v>
       </c>
       <c r="D6" t="n">
-        <v>0.944</v>
+        <v>0.8679</v>
       </c>
     </row>
     <row r="7">
@@ -2942,13 +2950,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.8607</v>
+        <v>-0.7947</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2697</v>
+        <v>0.2635</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0014</v>
+        <v>0.0026</v>
       </c>
     </row>
     <row r="8">
@@ -2956,13 +2964,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.2585</v>
+        <v>-0.2888</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2615</v>
+        <v>0.2533</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3228</v>
+        <v>0.2543</v>
       </c>
     </row>
     <row r="9">
@@ -2970,13 +2978,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.371</v>
+        <v>-0.3181</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3055</v>
+        <v>0.2973</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2247</v>
+        <v>0.2846</v>
       </c>
     </row>
     <row r="10">
@@ -2984,13 +2992,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.0467</v>
+        <v>-0.0263</v>
       </c>
       <c r="C10" t="n">
-        <v>0.244</v>
+        <v>0.2367</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8483</v>
+        <v>0.9114</v>
       </c>
     </row>
     <row r="11">
@@ -2998,13 +3006,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1698</v>
+        <v>0.1406</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2462</v>
+        <v>0.2384</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4903</v>
+        <v>0.5555</v>
       </c>
     </row>
     <row r="12">
@@ -3012,13 +3020,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.1988</v>
+        <v>-0.1911</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3693</v>
+        <v>0.3592</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5903</v>
+        <v>0.5947</v>
       </c>
     </row>
     <row r="13">
@@ -3026,13 +3034,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.3514</v>
+        <v>-0.3377</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5225</v>
+        <v>0.5081</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5012</v>
+        <v>0.5063</v>
       </c>
     </row>
     <row r="14">
@@ -3040,13 +3048,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.3049</v>
+        <v>-0.292</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5475</v>
+        <v>0.5321</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5776</v>
+        <v>0.5832</v>
       </c>
     </row>
     <row r="15">
@@ -3054,13 +3062,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.2741</v>
+        <v>-0.2599</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5375</v>
+        <v>0.5222</v>
       </c>
       <c r="D15" t="n">
-        <v>0.6102</v>
+        <v>0.6188</v>
       </c>
     </row>
     <row r="16">
@@ -3068,13 +3076,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.377</v>
+        <v>-0.3529</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5168</v>
+        <v>0.502</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4656</v>
+        <v>0.4822</v>
       </c>
     </row>
     <row r="17">
@@ -3082,13 +3090,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.4974</v>
+        <v>-0.4626</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5024</v>
+        <v>0.4881</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3221</v>
+        <v>0.3433</v>
       </c>
     </row>
     <row r="18">
@@ -3096,13 +3104,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.5668</v>
+        <v>-0.5216</v>
       </c>
       <c r="C18" t="n">
-        <v>0.4943</v>
+        <v>0.4803</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2515</v>
+        <v>0.2774</v>
       </c>
     </row>
     <row r="19">
@@ -3110,13 +3118,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.5785</v>
+        <v>-0.5281</v>
       </c>
       <c r="C19" t="n">
-        <v>0.4951</v>
+        <v>0.481</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2426</v>
+        <v>0.2722</v>
       </c>
     </row>
     <row r="20">
@@ -3124,13 +3132,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.6034</v>
+        <v>-0.556</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5139</v>
+        <v>0.4993</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2403</v>
+        <v>0.2655</v>
       </c>
     </row>
     <row r="21">
@@ -3138,13 +3146,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.48</v>
+        <v>-0.4393</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5251</v>
+        <v>0.5104</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3606</v>
+        <v>0.3893</v>
       </c>
     </row>
     <row r="22">
@@ -3152,13 +3160,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.2482</v>
+        <v>-0.2169</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5443</v>
+        <v>0.5292</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6485</v>
+        <v>0.6818</v>
       </c>
     </row>
     <row r="23">
@@ -3166,13 +3174,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.0144</v>
+        <v>0.0068</v>
       </c>
       <c r="C23" t="n">
-        <v>0.6974</v>
+        <v>0.6781</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9835</v>
+        <v>0.992</v>
       </c>
     </row>
     <row r="24">
@@ -3180,13 +3188,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.2332</v>
+        <v>-0.2728</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0734</v>
+        <v>0.073</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0015</v>
+        <v>0.0002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rearrange the parks alphabetically
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -42,13 +42,13 @@
     <t xml:space="preserve">AgeAdult</t>
   </si>
   <si>
+    <t xml:space="preserve">ParkEifel</t>
+  </si>
+  <si>
     <t xml:space="preserve">ParkHainich</t>
   </si>
   <si>
     <t xml:space="preserve">ParkHunsrueck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ParkSaechs_Schw</t>
   </si>
   <si>
     <t xml:space="preserve">ParkJasmund</t>
@@ -57,7 +57,7 @@
     <t xml:space="preserve">ParkKellerwald</t>
   </si>
   <si>
-    <t xml:space="preserve">ParkEifel</t>
+    <t xml:space="preserve">ParkSaechs_Schw</t>
   </si>
   <si>
     <t xml:space="preserve">ParkVorpomm</t>
@@ -450,10 +450,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4061</v>
+        <v>0.2467</v>
       </c>
       <c r="C2" t="n">
-        <v>31686.6893</v>
+        <v>85816.1197</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -492,10 +492,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>1.6647</v>
+        <v>1.7447</v>
       </c>
       <c r="C5" t="n">
-        <v>31686.6893</v>
+        <v>85816.1197</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -506,10 +506,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.2284</v>
+        <v>1.8242</v>
       </c>
       <c r="C6" t="n">
-        <v>40824.4892</v>
+        <v>85816.1197</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -519,39 +519,31 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="n">
-        <v>-0.2215</v>
-      </c>
+      <c r="B7"/>
       <c r="C7" t="n">
-        <v>38695.3832</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="n">
-        <v>-0.1344</v>
-      </c>
+      <c r="B8"/>
       <c r="C8" t="n">
-        <v>42715.2131</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>1.19</v>
+        <v>1.3494</v>
       </c>
       <c r="C9" t="n">
-        <v>31686.6893</v>
+        <v>85816.1197</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -561,29 +553,21 @@
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="n">
-        <v>1.5852</v>
-      </c>
+      <c r="B10"/>
       <c r="C10" t="n">
-        <v>31686.6893</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="n">
-        <v>-0.0641</v>
-      </c>
+      <c r="B11"/>
       <c r="C11" t="n">
-        <v>42580.1311</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -842,13 +826,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2237</v>
+        <v>-0.2778</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1549</v>
+        <v>0.1692</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1486</v>
+        <v>0.1006</v>
       </c>
     </row>
     <row r="6">
@@ -856,13 +840,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.5301</v>
+        <v>0.2237</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2023</v>
+        <v>0.1549</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0088</v>
+        <v>0.1486</v>
       </c>
     </row>
     <row r="7">
@@ -870,13 +854,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.241</v>
+        <v>-0.5301</v>
       </c>
       <c r="C7" t="n">
-        <v>0.147</v>
+        <v>0.2023</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1011</v>
+        <v>0.0088</v>
       </c>
     </row>
     <row r="8">
@@ -912,13 +896,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.2778</v>
+        <v>0.241</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1692</v>
+        <v>0.147</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1006</v>
+        <v>0.1011</v>
       </c>
     </row>
     <row r="11">
@@ -1192,13 +1176,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-4.1308</v>
+        <v>0.7964</v>
       </c>
       <c r="C5" t="n">
-        <v>31132.3064</v>
+        <v>0.4608</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9999</v>
+        <v>0.0839</v>
       </c>
     </row>
     <row r="6">
@@ -1206,13 +1190,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.1033</v>
+        <v>-4.1308</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5976</v>
+        <v>31132.3064</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8627</v>
+        <v>0.9999</v>
       </c>
     </row>
     <row r="7">
@@ -1220,13 +1204,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.3199</v>
+        <v>-0.1033</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4924</v>
+        <v>0.5976</v>
       </c>
       <c r="D7" t="n">
-        <v>0.516</v>
+        <v>0.8627</v>
       </c>
     </row>
     <row r="8">
@@ -1262,13 +1246,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.7964</v>
+        <v>0.3199</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4608</v>
+        <v>0.4924</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0839</v>
+        <v>0.516</v>
       </c>
     </row>
     <row r="11">
@@ -1542,13 +1526,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.0508</v>
+        <v>0.0062</v>
       </c>
       <c r="C5" t="n">
-        <v>0.09</v>
+        <v>0.0808</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5723</v>
+        <v>0.9385</v>
       </c>
     </row>
     <row r="6">
@@ -1556,13 +1540,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0425</v>
+        <v>-0.0508</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0822</v>
+        <v>0.09</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6055</v>
+        <v>0.5723</v>
       </c>
     </row>
     <row r="7">
@@ -1570,13 +1554,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.1305</v>
+        <v>0.0425</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0857</v>
+        <v>0.0822</v>
       </c>
       <c r="D7" t="n">
-        <v>0.128</v>
+        <v>0.6055</v>
       </c>
     </row>
     <row r="8">
@@ -1612,13 +1596,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0062</v>
+        <v>-0.1305</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0808</v>
+        <v>0.0857</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9385</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="11">
@@ -1892,13 +1876,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2732</v>
+        <v>0.5066</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4071</v>
+        <v>0.4029</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5022</v>
+        <v>0.2086</v>
       </c>
     </row>
     <row r="6">
@@ -1906,13 +1890,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3417</v>
+        <v>0.2732</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4097</v>
+        <v>0.4071</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4043</v>
+        <v>0.5022</v>
       </c>
     </row>
     <row r="7">
@@ -1920,13 +1904,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0394</v>
+        <v>0.3417</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4375</v>
+        <v>0.4097</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9282</v>
+        <v>0.4043</v>
       </c>
     </row>
     <row r="8">
@@ -1962,13 +1946,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.5066</v>
+        <v>0.0394</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4029</v>
+        <v>0.4375</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2086</v>
+        <v>0.9282</v>
       </c>
     </row>
     <row r="11">
@@ -2242,13 +2226,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.3065</v>
+        <v>0.2152</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2529</v>
+        <v>0.1585</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2254</v>
+        <v>0.1745</v>
       </c>
     </row>
     <row r="6">
@@ -2256,13 +2240,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2063</v>
+        <v>-0.3065</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1625</v>
+        <v>0.2529</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2041</v>
+        <v>0.2254</v>
       </c>
     </row>
     <row r="7">
@@ -2270,13 +2254,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.061</v>
+        <v>0.2063</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1622</v>
+        <v>0.1625</v>
       </c>
       <c r="D7" t="n">
-        <v>0.707</v>
+        <v>0.2041</v>
       </c>
     </row>
     <row r="8">
@@ -2312,13 +2296,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2152</v>
+        <v>0.061</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1585</v>
+        <v>0.1622</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1745</v>
+        <v>0.707</v>
       </c>
     </row>
     <row r="11">
@@ -2592,13 +2576,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.607</v>
+        <v>0.1365</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5845</v>
+        <v>0.6849</v>
       </c>
       <c r="D5" t="n">
-        <v>0.299</v>
+        <v>0.842</v>
       </c>
     </row>
     <row r="6">
@@ -2606,13 +2590,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.2895</v>
+        <v>0.607</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7234</v>
+        <v>0.5845</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6891</v>
+        <v>0.299</v>
       </c>
     </row>
     <row r="7">
@@ -2620,13 +2604,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-2.0377</v>
+        <v>-0.2895</v>
       </c>
       <c r="C7" t="n">
-        <v>2189.6613</v>
+        <v>0.7234</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9993</v>
+        <v>0.6891</v>
       </c>
     </row>
     <row r="8">
@@ -2662,13 +2646,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1365</v>
+        <v>-2.0377</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6849</v>
+        <v>2189.6613</v>
       </c>
       <c r="D10" t="n">
-        <v>0.842</v>
+        <v>0.9993</v>
       </c>
     </row>
     <row r="11">
@@ -2942,13 +2926,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.1329</v>
+        <v>-0.0263</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2392</v>
+        <v>0.2367</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5783</v>
+        <v>0.9114</v>
       </c>
     </row>
     <row r="6">
@@ -2956,13 +2940,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0402</v>
+        <v>-0.1329</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2417</v>
+        <v>0.2392</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8679</v>
+        <v>0.5783</v>
       </c>
     </row>
     <row r="7">
@@ -2970,13 +2954,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.7947</v>
+        <v>0.0402</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2635</v>
+        <v>0.2417</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0026</v>
+        <v>0.8679</v>
       </c>
     </row>
     <row r="8">
@@ -3012,13 +2996,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.0263</v>
+        <v>-0.7947</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2367</v>
+        <v>0.2635</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9114</v>
+        <v>0.0026</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Issue #70: Add the calculation of the confidence intervals to the files with results
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -31,6 +31,15 @@
   </si>
   <si>
     <t xml:space="preserve">p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimate_on_the_response_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lwr_on_the_response_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uppr_on_the_response_scale</t>
   </si>
   <si>
     <t xml:space="preserve">(Intercept)</t>
@@ -444,10 +453,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>0.2467</v>
@@ -458,10 +476,19 @@
       <c r="D2" t="n">
         <v>1</v>
       </c>
+      <c r="E2" t="n">
+        <v>1.2798</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>-0.2594</v>
@@ -472,10 +499,19 @@
       <c r="D3" t="n">
         <v>0.2453</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.7715</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.498</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.1951</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>-0.1332</v>
@@ -486,10 +522,19 @@
       <c r="D4" t="n">
         <v>0.4313</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.8753</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.6283</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.2195</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>1.7447</v>
@@ -500,10 +545,19 @@
       <c r="D5" t="n">
         <v>1</v>
       </c>
+      <c r="E5" t="n">
+        <v>5.7239</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>1.8242</v>
@@ -514,30 +568,45 @@
       <c r="D6" t="n">
         <v>1</v>
       </c>
+      <c r="E6" t="n">
+        <v>6.1975</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7"/>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>1.3494</v>
@@ -548,30 +617,45 @@
       <c r="D9" t="n">
         <v>1</v>
       </c>
+      <c r="E9" t="n">
+        <v>3.8551</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10"/>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.5778</v>
@@ -582,10 +666,19 @@
       <c r="D12" t="n">
         <v>0.3643</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.5611</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.161</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.9553</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-1.0665</v>
@@ -596,10 +689,19 @@
       <c r="D13" t="n">
         <v>0.218</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.3442</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0631</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.878</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-1.2398</v>
@@ -610,10 +712,19 @@
       <c r="D14" t="n">
         <v>0.1571</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.2895</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.6125</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-1.1869</v>
@@ -624,10 +735,19 @@
       <c r="D15" t="n">
         <v>0.1421</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.3052</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0626</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.4883</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>-1.0491</v>
@@ -638,10 +758,19 @@
       <c r="D16" t="n">
         <v>0.165</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.3503</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0797</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.5401</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>-0.8321</v>
@@ -652,10 +781,19 @@
       <c r="D17" t="n">
         <v>0.2434</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.4351</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.1075</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.761</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>-0.7644</v>
@@ -666,10 +804,19 @@
       <c r="D18" t="n">
         <v>0.2736</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.4656</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.1185</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.8297</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-0.9932</v>
@@ -680,10 +827,19 @@
       <c r="D19" t="n">
         <v>0.1547</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.3704</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0943</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.4546</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-1.1157</v>
@@ -694,10 +850,19 @@
       <c r="D20" t="n">
         <v>0.1406</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.3277</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0743</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.4452</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-1.1348</v>
@@ -708,10 +873,19 @@
       <c r="D21" t="n">
         <v>0.1823</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.3215</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0607</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.7041</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-1.1315</v>
@@ -722,10 +896,19 @@
       <c r="D22" t="n">
         <v>0.3256</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.3225</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0338</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3.0786</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>-1.1283</v>
@@ -736,10 +919,19 @@
       <c r="D23" t="n">
         <v>0.521</v>
       </c>
+      <c r="E23" t="n">
+        <v>0.3236</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0103</v>
+      </c>
+      <c r="G23" t="n">
+        <v>10.1497</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-1.225</v>
@@ -749,6 +941,15 @@
       </c>
       <c r="D24" t="n">
         <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2938</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.1902</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.4536</v>
       </c>
     </row>
   </sheetData>
@@ -778,10 +979,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>2.6353</v>
@@ -792,10 +1002,19 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>13.9481</v>
+      </c>
+      <c r="F2" t="n">
+        <v>6.8806</v>
+      </c>
+      <c r="G2" t="n">
+        <v>28.2752</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>0.1302</v>
@@ -806,10 +1025,19 @@
       <c r="D3" t="n">
         <v>0.1586</v>
       </c>
+      <c r="E3" t="n">
+        <v>1.1391</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9504</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.3651</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>0.0416</v>
@@ -820,10 +1048,19 @@
       <c r="D4" t="n">
         <v>0.6332</v>
       </c>
+      <c r="E4" t="n">
+        <v>1.0424</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8788</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.2365</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>-0.2778</v>
@@ -834,10 +1071,19 @@
       <c r="D5" t="n">
         <v>0.1006</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.7575</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.5437</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.0553</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>0.2237</v>
@@ -848,10 +1094,19 @@
       <c r="D6" t="n">
         <v>0.1486</v>
       </c>
+      <c r="E6" t="n">
+        <v>1.2508</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.9233</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.6944</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>-0.5301</v>
@@ -862,10 +1117,19 @@
       <c r="D7" t="n">
         <v>0.0088</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.5885</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.3959</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>0.3141</v>
@@ -876,10 +1140,19 @@
       <c r="D8" t="n">
         <v>0.0424</v>
       </c>
+      <c r="E8" t="n">
+        <v>1.369</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.0108</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.8541</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>-0.3997</v>
@@ -890,10 +1163,19 @@
       <c r="D9" t="n">
         <v>0.0634</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.6705</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4396</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.0226</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>0.241</v>
@@ -904,10 +1186,19 @@
       <c r="D10" t="n">
         <v>0.1011</v>
       </c>
+      <c r="E10" t="n">
+        <v>1.2726</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.954</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.6975</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>-0.1211</v>
@@ -918,10 +1209,19 @@
       <c r="D11" t="n">
         <v>0.4696</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.886</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6381</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.2301</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.2446</v>
@@ -932,10 +1232,19 @@
       <c r="D12" t="n">
         <v>0.3288</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.4792</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.2793</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-0.4456</v>
@@ -946,10 +1255,19 @@
       <c r="D13" t="n">
         <v>0.2137</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.6404</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.3173</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.2927</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-0.5311</v>
@@ -960,10 +1278,19 @@
       <c r="D14" t="n">
         <v>0.161</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.588</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.2798</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.2356</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-0.5908</v>
@@ -974,10 +1301,19 @@
       <c r="D15" t="n">
         <v>0.1148</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.5539</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.2658</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.1542</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>-0.5513</v>
@@ -988,10 +1324,19 @@
       <c r="D16" t="n">
         <v>0.1282</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.5762</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.2832</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.1724</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>-0.4823</v>
@@ -1002,10 +1347,19 @@
       <c r="D17" t="n">
         <v>0.1664</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.6174</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.3118</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.2224</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>-0.4713</v>
@@ -1016,10 +1370,19 @@
       <c r="D18" t="n">
         <v>0.1661</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.6242</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.3203</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.2163</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-0.5076</v>
@@ -1030,10 +1393,19 @@
       <c r="D19" t="n">
         <v>0.1359</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.602</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.3089</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.173</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-0.4477</v>
@@ -1044,10 +1416,19 @@
       <c r="D20" t="n">
         <v>0.1991</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.6391</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.3227</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.2656</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-0.3903</v>
@@ -1058,10 +1439,19 @@
       <c r="D21" t="n">
         <v>0.2663</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.6768</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.3401</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.3471</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-0.555</v>
@@ -1072,10 +1462,19 @@
       <c r="D22" t="n">
         <v>0.1178</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.5741</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.2864</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.1508</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>-0.7725</v>
@@ -1086,10 +1485,19 @@
       <c r="D23" t="n">
         <v>0.0811</v>
       </c>
+      <c r="E23" t="n">
+        <v>0.4618</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.1939</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.1003</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-0.6532</v>
@@ -1099,6 +1507,15 @@
       </c>
       <c r="D24" t="n">
         <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.5204</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.4637</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.584</v>
       </c>
     </row>
   </sheetData>
@@ -1128,10 +1545,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>0.6536</v>
@@ -1142,10 +1568,19 @@
       <c r="D2" t="n">
         <v>0.584</v>
       </c>
+      <c r="E2" t="n">
+        <v>1.9225</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.1853</v>
+      </c>
+      <c r="G2" t="n">
+        <v>19.9503</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>-0.2104</v>
@@ -1156,10 +1591,19 @@
       <c r="D3" t="n">
         <v>0.4523</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.8103</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.4681</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.4025</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>-0.1423</v>
@@ -1170,10 +1614,19 @@
       <c r="D4" t="n">
         <v>0.6125</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.8674</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.5001</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.5043</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>0.7964</v>
@@ -1184,10 +1637,19 @@
       <c r="D5" t="n">
         <v>0.0839</v>
       </c>
+      <c r="E5" t="n">
+        <v>2.2176</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.8987</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5.4718</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>-4.1308</v>
@@ -1198,10 +1660,19 @@
       <c r="D6" t="n">
         <v>0.9999</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.0161</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>-0.1033</v>
@@ -1212,10 +1683,19 @@
       <c r="D7" t="n">
         <v>0.8627</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.9018</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.2795</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2.9096</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>-4.2098</v>
@@ -1226,10 +1706,19 @@
       <c r="D8" t="n">
         <v>0.9999</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.0148</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>-3.3352</v>
@@ -1240,10 +1729,19 @@
       <c r="D9" t="n">
         <v>0.9999</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.0356</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>0.3199</v>
@@ -1254,10 +1752,19 @@
       <c r="D10" t="n">
         <v>0.516</v>
       </c>
+      <c r="E10" t="n">
+        <v>1.3769</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.5245</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3.6145</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>-0.3848</v>
@@ -1268,10 +1775,19 @@
       <c r="D11" t="n">
         <v>0.5567</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.6806</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.1887</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2.4553</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.1796</v>
@@ -1282,10 +1798,19 @@
       <c r="D12" t="n">
         <v>0.8304</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.8356</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.1616</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4.3206</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-0.3215</v>
@@ -1296,10 +1821,19 @@
       <c r="D13" t="n">
         <v>0.7917</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0667</v>
+      </c>
+      <c r="G13" t="n">
+        <v>7.8782</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-0.2983</v>
@@ -1310,10 +1844,19 @@
       <c r="D14" t="n">
         <v>0.8178</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.7421</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0586</v>
+      </c>
+      <c r="G14" t="n">
+        <v>9.3895</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-0.0764</v>
@@ -1324,10 +1867,19 @@
       <c r="D15" t="n">
         <v>0.9519</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.9264</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0776</v>
+      </c>
+      <c r="G15" t="n">
+        <v>11.0659</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>0.2627</v>
@@ -1338,10 +1890,19 @@
       <c r="D16" t="n">
         <v>0.8242</v>
       </c>
+      <c r="E16" t="n">
+        <v>1.3005</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.128</v>
+      </c>
+      <c r="G16" t="n">
+        <v>13.2141</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>0.6006</v>
@@ -1352,10 +1913,19 @@
       <c r="D17" t="n">
         <v>0.5952</v>
       </c>
+      <c r="E17" t="n">
+        <v>1.8232</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.199</v>
+      </c>
+      <c r="G17" t="n">
+        <v>16.7071</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>0.797</v>
@@ -1366,10 +1936,19 @@
       <c r="D18" t="n">
         <v>0.4761</v>
       </c>
+      <c r="E18" t="n">
+        <v>2.219</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.2478</v>
+      </c>
+      <c r="G18" t="n">
+        <v>19.8728</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>0.3992</v>
@@ -1380,10 +1959,19 @@
       <c r="D19" t="n">
         <v>0.7213</v>
       </c>
+      <c r="E19" t="n">
+        <v>1.4906</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.1663</v>
+      </c>
+      <c r="G19" t="n">
+        <v>13.3622</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>0.0343</v>
@@ -1394,10 +1982,19 @@
       <c r="D20" t="n">
         <v>0.9764</v>
       </c>
+      <c r="E20" t="n">
+        <v>1.0348</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.1067</v>
+      </c>
+      <c r="G20" t="n">
+        <v>10.0359</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>0.0067</v>
@@ -1408,10 +2005,19 @@
       <c r="D21" t="n">
         <v>0.9955</v>
       </c>
+      <c r="E21" t="n">
+        <v>1.0067</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.1002</v>
+      </c>
+      <c r="G21" t="n">
+        <v>10.1188</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>0.2032</v>
@@ -1422,10 +2028,19 @@
       <c r="D22" t="n">
         <v>0.8616</v>
       </c>
+      <c r="E22" t="n">
+        <v>1.2253</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.1248</v>
+      </c>
+      <c r="G22" t="n">
+        <v>12.0323</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>0.4415</v>
@@ -1436,10 +2051,19 @@
       <c r="D23" t="n">
         <v>0.7602</v>
       </c>
+      <c r="E23" t="n">
+        <v>1.555</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0913</v>
+      </c>
+      <c r="G23" t="n">
+        <v>26.4917</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-0.2729</v>
@@ -1449,6 +2073,15 @@
       </c>
       <c r="D24" t="n">
         <v>0.032</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.7612</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.5932</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.9768</v>
       </c>
     </row>
   </sheetData>
@@ -1478,10 +2111,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>2.8062</v>
@@ -1492,10 +2134,19 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>16.5472</v>
+      </c>
+      <c r="F2" t="n">
+        <v>11.6429</v>
+      </c>
+      <c r="G2" t="n">
+        <v>23.5174</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>0.0303</v>
@@ -1506,10 +2157,19 @@
       <c r="D3" t="n">
         <v>0.5363</v>
       </c>
+      <c r="E3" t="n">
+        <v>1.0307</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9364</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.1346</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>0.0409</v>
@@ -1520,10 +2180,19 @@
       <c r="D4" t="n">
         <v>0.3729</v>
       </c>
+      <c r="E4" t="n">
+        <v>1.0417</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9521</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.1398</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>0.0062</v>
@@ -1534,10 +2203,19 @@
       <c r="D5" t="n">
         <v>0.9385</v>
       </c>
+      <c r="E5" t="n">
+        <v>1.0063</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.8588</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.179</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>-0.0508</v>
@@ -1548,10 +2226,19 @@
       <c r="D6" t="n">
         <v>0.5723</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.9504</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.7967</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.1339</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>0.0425</v>
@@ -1562,10 +2249,19 @@
       <c r="D7" t="n">
         <v>0.6055</v>
       </c>
+      <c r="E7" t="n">
+        <v>1.0434</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.8881</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.2259</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>-0.0705</v>
@@ -1576,10 +2272,19 @@
       <c r="D8" t="n">
         <v>0.448</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.9319</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.7768</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.1181</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>-0.1751</v>
@@ -1590,10 +2295,19 @@
       <c r="D9" t="n">
         <v>0.0948</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.8394</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.6835</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.0308</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>-0.1305</v>
@@ -1604,10 +2318,19 @@
       <c r="D10" t="n">
         <v>0.128</v>
       </c>
+      <c r="E10" t="n">
+        <v>0.8777</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.7419</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.0383</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>-0.1154</v>
@@ -1618,10 +2341,19 @@
       <c r="D11" t="n">
         <v>0.2155</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.891</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.7423</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.0695</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.0717</v>
@@ -1632,10 +2364,19 @@
       <c r="D12" t="n">
         <v>0.5758</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.9308</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.7241</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.1965</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-0.1335</v>
@@ -1646,10 +2387,19 @@
       <c r="D13" t="n">
         <v>0.4565</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.6158</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.2434</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-0.15</v>
@@ -1660,10 +2410,19 @@
       <c r="D14" t="n">
         <v>0.4216</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.8607</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.597</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.2408</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-0.1739</v>
@@ -1674,10 +2433,19 @@
       <c r="D15" t="n">
         <v>0.3419</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.8404</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.5871</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.2029</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>-0.2197</v>
@@ -1688,10 +2456,19 @@
       <c r="D16" t="n">
         <v>0.2106</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.8027</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.5691</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.1323</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>-0.2461</v>
@@ -1702,10 +2479,19 @@
       <c r="D17" t="n">
         <v>0.1487</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.7818</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.5598</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.0919</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>-0.2325</v>
@@ -1716,10 +2502,19 @@
       <c r="D18" t="n">
         <v>0.1632</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.7925</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.5716</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.0989</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-0.1979</v>
@@ -1730,10 +2525,19 @@
       <c r="D19" t="n">
         <v>0.234</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.8205</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.5923</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.1365</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-0.1916</v>
@@ -1744,10 +2548,19 @@
       <c r="D20" t="n">
         <v>0.2678</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.8256</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.5883</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.1587</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-0.2</v>
@@ -1758,10 +2571,19 @@
       <c r="D21" t="n">
         <v>0.2585</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.8187</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.5787</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.1583</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-0.1708</v>
@@ -1772,10 +2594,19 @@
       <c r="D22" t="n">
         <v>0.3462</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.843</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.5908</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.2028</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>-0.1306</v>
@@ -1786,10 +2617,19 @@
       <c r="D23" t="n">
         <v>0.5759</v>
       </c>
+      <c r="E23" t="n">
+        <v>0.8775</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.5552</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.3869</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-1.5118</v>
@@ -1799,6 +2639,15 @@
       </c>
       <c r="D24" t="n">
         <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2205</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.1886</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.2578</v>
       </c>
     </row>
   </sheetData>
@@ -1828,10 +2677,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>3.6956</v>
@@ -1842,10 +2700,19 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>40.2687</v>
+      </c>
+      <c r="F2" t="n">
+        <v>13.6576</v>
+      </c>
+      <c r="G2" t="n">
+        <v>118.7305</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>0.0617</v>
@@ -1856,10 +2723,19 @@
       <c r="D3" t="n">
         <v>0.5074</v>
       </c>
+      <c r="E3" t="n">
+        <v>1.0637</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8862</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.2766</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>-0.0038</v>
@@ -1870,10 +2746,19 @@
       <c r="D4" t="n">
         <v>0.9695</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.9962</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8201</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.2101</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>0.5066</v>
@@ -1884,10 +2769,19 @@
       <c r="D5" t="n">
         <v>0.2086</v>
       </c>
+      <c r="E5" t="n">
+        <v>1.6597</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.7535</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3.6557</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>0.2732</v>
@@ -1898,10 +2792,19 @@
       <c r="D6" t="n">
         <v>0.5022</v>
       </c>
+      <c r="E6" t="n">
+        <v>1.3141</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5917</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2.9184</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>0.3417</v>
@@ -1912,10 +2815,19 @@
       <c r="D7" t="n">
         <v>0.4043</v>
       </c>
+      <c r="E7" t="n">
+        <v>1.4074</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.6305</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.1416</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>-0.0368</v>
@@ -1926,10 +2838,19 @@
       <c r="D8" t="n">
         <v>0.9422</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.9639</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.3561</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2.6086</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>0.0543</v>
@@ -1940,10 +2861,19 @@
       <c r="D9" t="n">
         <v>0.9074</v>
       </c>
+      <c r="E9" t="n">
+        <v>1.0558</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4228</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2.6367</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>0.0394</v>
@@ -1954,10 +2884,19 @@
       <c r="D10" t="n">
         <v>0.9282</v>
       </c>
+      <c r="E10" t="n">
+        <v>1.0402</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.4413</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2.4519</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>0.2517</v>
@@ -1968,10 +2907,19 @@
       <c r="D11" t="n">
         <v>0.5363</v>
       </c>
+      <c r="E11" t="n">
+        <v>1.2862</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.5792</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2.8563</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.3645</v>
@@ -1982,10 +2930,19 @@
       <c r="D12" t="n">
         <v>0.2739</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.6946</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.3615</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.3344</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-0.6841</v>
@@ -1996,10 +2953,19 @@
       <c r="D13" t="n">
         <v>0.1382</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.5046</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.2043</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.2464</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-0.7966</v>
@@ -2010,10 +2976,19 @@
       <c r="D14" t="n">
         <v>0.0989</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.4509</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.1614</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-0.7271</v>
@@ -2024,10 +2999,19 @@
       <c r="D15" t="n">
         <v>0.1147</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.4833</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.1958</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.1929</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>-0.5878</v>
@@ -2038,10 +3022,19 @@
       <c r="D16" t="n">
         <v>0.158</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.5555</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.2457</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.2563</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>-0.4762</v>
@@ -2052,10 +3045,19 @@
       <c r="D17" t="n">
         <v>0.2243</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.6211</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.2881</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.339</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>-0.4278</v>
@@ -2066,10 +3068,19 @@
       <c r="D18" t="n">
         <v>0.2673</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.3062</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.3883</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-0.4209</v>
@@ -2080,10 +3091,19 @@
       <c r="D19" t="n">
         <v>0.2753</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.6564</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.3082</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.3983</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-0.4618</v>
@@ -2094,10 +3114,19 @@
       <c r="D20" t="n">
         <v>0.2587</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.6301</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.2827</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.4044</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-0.5497</v>
@@ -2108,10 +3137,19 @@
       <c r="D21" t="n">
         <v>0.2203</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.5771</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.2396</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.39</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-0.6302</v>
@@ -2122,10 +3160,19 @@
       <c r="D22" t="n">
         <v>0.2575</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.5325</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.1789</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.5852</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>-0.7091</v>
@@ -2136,10 +3183,19 @@
       <c r="D23" t="n">
         <v>0.3812</v>
       </c>
+      <c r="E23" t="n">
+        <v>0.4921</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.1006</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2.406</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-1.2996</v>
@@ -2149,6 +3205,15 @@
       </c>
       <c r="D24" t="n">
         <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2726</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.2088</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.356</v>
       </c>
     </row>
   </sheetData>
@@ -2178,10 +3243,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>2.315</v>
@@ -2192,10 +3266,19 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>10.1249</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5.8048</v>
+      </c>
+      <c r="G2" t="n">
+        <v>17.66</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>-0.2653</v>
@@ -2206,10 +3289,19 @@
       <c r="D3" t="n">
         <v>0.0012</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.6535</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9002</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>-0.3223</v>
@@ -2220,10 +3312,19 @@
       <c r="D4" t="n">
         <v>0.0003</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.7245</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.6092</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.8615</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>0.2152</v>
@@ -2234,10 +3335,19 @@
       <c r="D5" t="n">
         <v>0.1745</v>
       </c>
+      <c r="E5" t="n">
+        <v>1.2401</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.909</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.6919</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>-0.3065</v>
@@ -2248,10 +3358,19 @@
       <c r="D6" t="n">
         <v>0.2254</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.736</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.4484</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.2081</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>0.2063</v>
@@ -2262,10 +3381,19 @@
       <c r="D7" t="n">
         <v>0.2041</v>
       </c>
+      <c r="E7" t="n">
+        <v>1.2292</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.8939</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.6901</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>-0.4051</v>
@@ -2276,10 +3404,19 @@
       <c r="D8" t="n">
         <v>0.2362</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.6669</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.3412</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.3037</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>0.3051</v>
@@ -2290,10 +3427,19 @@
       <c r="D9" t="n">
         <v>0.0836</v>
       </c>
+      <c r="E9" t="n">
+        <v>1.3568</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.9602</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.917</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>0.061</v>
@@ -2304,10 +3450,19 @@
       <c r="D10" t="n">
         <v>0.707</v>
       </c>
+      <c r="E10" t="n">
+        <v>1.0629</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.7734</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.4607</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>-0.4734</v>
@@ -2318,10 +3473,19 @@
       <c r="D11" t="n">
         <v>0.3575</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.6229</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.2272</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.7073</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.0528</v>
@@ -2332,10 +3496,19 @@
       <c r="D12" t="n">
         <v>0.7886</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.9486</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.6449</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.3952</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-0.0986</v>
@@ -2346,10 +3519,19 @@
       <c r="D13" t="n">
         <v>0.7109</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.9061</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.5381</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.5258</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-0.1032</v>
@@ -2360,10 +3542,19 @@
       <c r="D14" t="n">
         <v>0.7043</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.902</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.5295</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.5365</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-0.0517</v>
@@ -2374,10 +3565,19 @@
       <c r="D15" t="n">
         <v>0.847</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.9497</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.5618</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.6051</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>0.0129</v>
@@ -2388,10 +3588,19 @@
       <c r="D16" t="n">
         <v>0.9599</v>
       </c>
+      <c r="E16" t="n">
+        <v>1.0129</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.6134</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.6726</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>0.0513</v>
@@ -2402,10 +3611,19 @@
       <c r="D17" t="n">
         <v>0.8379</v>
       </c>
+      <c r="E17" t="n">
+        <v>1.0526</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.6441</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.7203</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>0.0151</v>
@@ -2416,10 +3634,19 @@
       <c r="D18" t="n">
         <v>0.9516</v>
       </c>
+      <c r="E18" t="n">
+        <v>1.0152</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.6236</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.6528</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-0.0803</v>
@@ -2430,10 +3657,19 @@
       <c r="D19" t="n">
         <v>0.7466</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.9229</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.5671</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.5018</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-0.1165</v>
@@ -2444,10 +3680,19 @@
       <c r="D20" t="n">
         <v>0.6586</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.5308</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.4923</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-0.0855</v>
@@ -2458,10 +3703,19 @@
       <c r="D21" t="n">
         <v>0.7547</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.9181</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.5371</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.5693</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-0.0216</v>
@@ -2472,10 +3726,19 @@
       <c r="D22" t="n">
         <v>0.9396</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.9786</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.5596</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.7113</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>0.048</v>
@@ -2486,10 +3749,19 @@
       <c r="D23" t="n">
         <v>0.9003</v>
       </c>
+      <c r="E23" t="n">
+        <v>1.0492</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.4951</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2.2232</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-1.3513</v>
@@ -2499,6 +3771,15 @@
       </c>
       <c r="D24" t="n">
         <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2589</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.2207</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.3037</v>
       </c>
     </row>
   </sheetData>
@@ -2528,10 +3809,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>3.3025</v>
@@ -2542,10 +3832,19 @@
       <c r="D2" t="n">
         <v>0.0099</v>
       </c>
+      <c r="E2" t="n">
+        <v>27.1793</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2.2101</v>
+      </c>
+      <c r="G2" t="n">
+        <v>334.2463</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>0.5262</v>
@@ -2556,10 +3855,19 @@
       <c r="D3" t="n">
         <v>0.0303</v>
       </c>
+      <c r="E3" t="n">
+        <v>1.6924</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.0513</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.7247</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>0.3542</v>
@@ -2570,10 +3878,19 @@
       <c r="D4" t="n">
         <v>0.1285</v>
       </c>
+      <c r="E4" t="n">
+        <v>1.425</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9025</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.2501</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>0.1365</v>
@@ -2584,10 +3901,19 @@
       <c r="D5" t="n">
         <v>0.842</v>
       </c>
+      <c r="E5" t="n">
+        <v>1.1463</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.2994</v>
+      </c>
+      <c r="G5" t="n">
+        <v>4.3885</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>0.607</v>
@@ -2598,10 +3924,19 @@
       <c r="D6" t="n">
         <v>0.299</v>
       </c>
+      <c r="E6" t="n">
+        <v>1.8349</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5836</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5.7691</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>-0.2895</v>
@@ -2612,10 +3947,19 @@
       <c r="D7" t="n">
         <v>0.6891</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.7487</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.1813</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.0907</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>0.6646</v>
@@ -2626,10 +3970,19 @@
       <c r="D8" t="n">
         <v>0.2402</v>
       </c>
+      <c r="E8" t="n">
+        <v>1.9438</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.6411</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5.8934</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>-0.4127</v>
@@ -2640,10 +3993,19 @@
       <c r="D9" t="n">
         <v>0.5945</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.6618</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.1448</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3.0243</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>-2.0377</v>
@@ -2654,10 +4016,19 @@
       <c r="D10" t="n">
         <v>0.9993</v>
       </c>
+      <c r="E10" t="n">
+        <v>0.1303</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>-1.4508</v>
@@ -2668,10 +4039,19 @@
       <c r="D11" t="n">
         <v>0.9996</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.2344</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-1.2623</v>
@@ -2682,10 +4062,19 @@
       <c r="D12" t="n">
         <v>0.1951</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.283</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0419</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.9104</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-2.3668</v>
@@ -2696,10 +4085,19 @@
       <c r="D13" t="n">
         <v>0.1062</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.0938</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0053</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.656</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-2.9957</v>
@@ -2710,10 +4108,19 @@
       <c r="D14" t="n">
         <v>0.0813</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0017</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.4513</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-3.2126</v>
@@ -2724,10 +4131,19 @@
       <c r="D15" t="n">
         <v>0.0655</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.0403</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0013</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.2282</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>-3.1079</v>
@@ -2738,10 +4154,19 @@
       <c r="D16" t="n">
         <v>0.0469</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.0447</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0021</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.9579</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>-2.7713</v>
@@ -2752,10 +4177,19 @@
       <c r="D17" t="n">
         <v>0.0332</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.0626</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0049</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.8019</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>-2.2698</v>
@@ -2766,10 +4200,19 @@
       <c r="D18" t="n">
         <v>0.0468</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.1033</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.9684</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-2.1592</v>
@@ -2780,10 +4223,19 @@
       <c r="D19" t="n">
         <v>0.0564</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.1154</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.0606</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-2.2244</v>
@@ -2794,10 +4246,19 @@
       <c r="D20" t="n">
         <v>0.0572</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.1081</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0109</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.0705</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-2.0845</v>
@@ -2808,10 +4269,19 @@
       <c r="D21" t="n">
         <v>0.0791</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.1244</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0121</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.2738</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-2.3118</v>
@@ -2822,10 +4292,19 @@
       <c r="D22" t="n">
         <v>0.0578</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.0991</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0091</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.0795</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>-2.6108</v>
@@ -2836,10 +4315,19 @@
       <c r="D23" t="n">
         <v>0.0875</v>
       </c>
+      <c r="E23" t="n">
+        <v>0.0735</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0037</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.4684</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-0.9765</v>
@@ -2849,6 +4337,15 @@
       </c>
       <c r="D24" t="n">
         <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.3766</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.2514</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.5643</v>
       </c>
     </row>
   </sheetData>
@@ -2878,10 +4375,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>3.27</v>
@@ -2892,10 +4398,19 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>26.3105</v>
+      </c>
+      <c r="F2" t="n">
+        <v>9.6939</v>
+      </c>
+      <c r="G2" t="n">
+        <v>71.41</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>-0.0697</v>
@@ -2906,10 +4421,19 @@
       <c r="D3" t="n">
         <v>0.64</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.9326</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.6963</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.2493</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>0.2093</v>
@@ -2920,10 +4444,19 @@
       <c r="D4" t="n">
         <v>0.1044</v>
       </c>
+      <c r="E4" t="n">
+        <v>1.2329</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9576</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.5873</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>-0.0263</v>
@@ -2934,10 +4467,19 @@
       <c r="D5" t="n">
         <v>0.9114</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.974</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.6125</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.5489</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>-0.1329</v>
@@ -2948,10 +4490,19 @@
       <c r="D6" t="n">
         <v>0.5783</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.8755</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5479</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.3991</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>0.0402</v>
@@ -2962,10 +4513,19 @@
       <c r="D7" t="n">
         <v>0.8679</v>
       </c>
+      <c r="E7" t="n">
+        <v>1.041</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.6482</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.6718</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>-0.2888</v>
@@ -2976,10 +4536,19 @@
       <c r="D8" t="n">
         <v>0.2543</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.7492</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.456</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.2309</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>-0.3181</v>
@@ -2990,10 +4559,19 @@
       <c r="D9" t="n">
         <v>0.2846</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.7275</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4062</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.3029</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>-0.7947</v>
@@ -3004,10 +4582,19 @@
       <c r="D10" t="n">
         <v>0.0026</v>
       </c>
+      <c r="E10" t="n">
+        <v>0.4517</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.2695</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.7571</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>0.1406</v>
@@ -3018,10 +4605,19 @@
       <c r="D11" t="n">
         <v>0.5555</v>
       </c>
+      <c r="E11" t="n">
+        <v>1.1509</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.7212</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.8366</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.1911</v>
@@ -3032,10 +4628,19 @@
       <c r="D12" t="n">
         <v>0.5947</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.826</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.4085</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.6701</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-0.3377</v>
@@ -3046,10 +4651,19 @@
       <c r="D13" t="n">
         <v>0.5063</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.7134</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.2636</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.9312</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-0.292</v>
@@ -3060,10 +4674,19 @@
       <c r="D14" t="n">
         <v>0.5832</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.7468</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.2632</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2.1189</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-0.2599</v>
@@ -3074,10 +4697,19 @@
       <c r="D15" t="n">
         <v>0.6188</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.7712</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.2771</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2.1462</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>-0.3529</v>
@@ -3088,10 +4720,19 @@
       <c r="D16" t="n">
         <v>0.4822</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.7027</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.2627</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.8797</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>-0.4626</v>
@@ -3102,10 +4743,19 @@
       <c r="D17" t="n">
         <v>0.3433</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.6297</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.2419</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.6391</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>-0.5216</v>
@@ -3116,10 +4766,19 @@
       <c r="D18" t="n">
         <v>0.2774</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.5935</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.2316</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.5214</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-0.5281</v>
@@ -3130,10 +4789,19 @@
       <c r="D19" t="n">
         <v>0.2722</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.5897</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.2297</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.5139</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-0.556</v>
@@ -3144,10 +4812,19 @@
       <c r="D20" t="n">
         <v>0.2655</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.5735</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.2156</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.526</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-0.4393</v>
@@ -3158,10 +4835,19 @@
       <c r="D21" t="n">
         <v>0.3893</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.6445</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.7524</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-0.2169</v>
@@ -3172,10 +4858,19 @@
       <c r="D22" t="n">
         <v>0.6818</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.2853</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2.271</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>0.0068</v>
@@ -3186,10 +4881,19 @@
       <c r="D23" t="n">
         <v>0.992</v>
       </c>
+      <c r="E23" t="n">
+        <v>1.0068</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.2665</v>
+      </c>
+      <c r="G23" t="n">
+        <v>3.8036</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-0.2728</v>
@@ -3199,6 +4903,15 @@
       </c>
       <c r="D24" t="n">
         <v>0.0002</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.7612</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.6598</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.8783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #77: Remove the 1e-6 regularization for zero values
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -471,7 +471,7 @@
         <v>0.2467</v>
       </c>
       <c r="C2" t="n">
-        <v>85816.1197</v>
+        <v>85835.7724</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -537,16 +537,16 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>1.7447</v>
+        <v>1.7446</v>
       </c>
       <c r="C5" t="n">
-        <v>85816.1197</v>
+        <v>85835.7724</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>5.7239</v>
+        <v>5.7236</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -560,16 +560,16 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>1.8242</v>
+        <v>1.8241</v>
       </c>
       <c r="C6" t="n">
-        <v>85816.1197</v>
+        <v>85835.7724</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>6.1975</v>
+        <v>6.1972</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -609,16 +609,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>1.3494</v>
+        <v>1.3493</v>
       </c>
       <c r="C9" t="n">
-        <v>85816.1197</v>
+        <v>85835.7724</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>3.8551</v>
+        <v>3.8549</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>

</xml_diff>